<commit_message>
working on Thursday schedules fix
</commit_message>
<xml_diff>
--- a/data/horarios/all.processed.xlsx
+++ b/data/horarios/all.processed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F740E869-AD98-4595-A85D-0AAFD143C1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901FF36D-73B6-423E-B575-90699677F37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2848" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2861" uniqueCount="1110">
   <si>
     <t>ciclo</t>
   </si>
@@ -3360,6 +3360,9 @@
   </si>
   <si>
     <t>C3S2A333</t>
+  </si>
+  <si>
+    <t>C3P22314</t>
   </si>
 </sst>
 </file>
@@ -3375,7 +3378,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3412,6 +3415,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3425,7 +3434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3450,6 +3459,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3523,11 +3536,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R256" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="A1:R256" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}">
-    <filterColumn colId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R257" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="A1:R257" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}">
+    <filterColumn colId="1">
       <filters>
-        <filter val="LUNES"/>
+        <filter val="PST"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="METODOLOGIA Y DISEÑO DE LA INVESTIGACION"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3833,10 +3851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R256"/>
+  <dimension ref="A1:R257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="J66" sqref="J66:J177"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A257" sqref="A257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7187,7 +7205,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>1</v>
       </c>
@@ -7289,7 +7307,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>1</v>
       </c>
@@ -7544,7 +7562,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2</v>
       </c>
@@ -7799,7 +7817,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>3</v>
       </c>
@@ -7901,7 +7919,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>4</v>
       </c>
@@ -7952,7 +7970,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>4</v>
       </c>
@@ -8207,7 +8225,7 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>1</v>
       </c>
@@ -8615,7 +8633,7 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>3</v>
       </c>
@@ -8666,7 +8684,7 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>3</v>
       </c>
@@ -8921,7 +8939,7 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>4</v>
       </c>
@@ -8972,7 +8990,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>4</v>
       </c>
@@ -9125,7 +9143,7 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>1</v>
       </c>
@@ -9176,7 +9194,7 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>1</v>
       </c>
@@ -9380,7 +9398,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>2</v>
       </c>
@@ -9431,7 +9449,7 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>2</v>
       </c>
@@ -9686,7 +9704,7 @@
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
     </row>
-    <row r="115" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>3</v>
       </c>
@@ -9788,7 +9806,7 @@
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
     </row>
-    <row r="117" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>3</v>
       </c>
@@ -9890,7 +9908,7 @@
       <c r="Q118" s="2"/>
       <c r="R118" s="2"/>
     </row>
-    <row r="119" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>4</v>
       </c>
@@ -9941,7 +9959,7 @@
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
     </row>
-    <row r="120" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>4</v>
       </c>
@@ -10094,7 +10112,7 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="1:18" ht="66" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" ht="66" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>1</v>
       </c>
@@ -10145,7 +10163,7 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>1</v>
       </c>
@@ -10298,7 +10316,7 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
     </row>
-    <row r="127" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>2</v>
       </c>
@@ -10451,7 +10469,7 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>2</v>
       </c>
@@ -10604,7 +10622,7 @@
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
     </row>
-    <row r="133" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>3</v>
       </c>
@@ -10655,7 +10673,7 @@
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
     </row>
-    <row r="134" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>3</v>
       </c>
@@ -10916,7 +10934,7 @@
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>4</v>
       </c>
@@ -12611,7 +12629,7 @@
       <c r="Q171" s="1"/>
       <c r="R171" s="1"/>
     </row>
-    <row r="172" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>3</v>
       </c>
@@ -12662,7 +12680,7 @@
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
     </row>
-    <row r="173" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>3</v>
       </c>
@@ -12866,7 +12884,7 @@
       <c r="Q176" s="1"/>
       <c r="R176" s="1"/>
     </row>
-    <row r="177" spans="1:18" ht="99" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:18" ht="99" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>4</v>
       </c>
@@ -15671,7 +15689,7 @@
       <c r="Q231" s="1"/>
       <c r="R231" s="1"/>
     </row>
-    <row r="232" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>1</v>
       </c>
@@ -15722,7 +15740,7 @@
       <c r="Q232" s="1"/>
       <c r="R232" s="1"/>
     </row>
-    <row r="233" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>1</v>
       </c>
@@ -16997,6 +17015,63 @@
         <v>1</v>
       </c>
       <c r="R256" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="257" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+      <c r="A257" s="10">
+        <v>1</v>
+      </c>
+      <c r="B257" s="10" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C257" s="10" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D257" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="E257" s="10">
+        <v>1</v>
+      </c>
+      <c r="F257" s="10" t="s">
+        <v>1031</v>
+      </c>
+      <c r="G257" s="10" t="s">
+        <v>1032</v>
+      </c>
+      <c r="H257" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="I257" s="10" t="s">
+        <v>1033</v>
+      </c>
+      <c r="J257" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K257" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L257" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M257" s="10" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N257" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O257" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P257" s="10" t="s">
+        <v>1030</v>
+      </c>
+      <c r="Q257" s="10">
+        <v>1</v>
+      </c>
+      <c r="R257" s="10" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
checking to many files of Thursday schedules
</commit_message>
<xml_diff>
--- a/data/horarios/all.processed.xlsx
+++ b/data/horarios/all.processed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901FF36D-73B6-423E-B575-90699677F37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78460894-EFE6-45EC-8930-86DBCF0C00DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2861" uniqueCount="1110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2965" uniqueCount="1113">
   <si>
     <t>ciclo</t>
   </si>
@@ -3363,6 +3363,15 @@
   </si>
   <si>
     <t>C3P22314</t>
+  </si>
+  <si>
+    <t>C3P21334</t>
+  </si>
+  <si>
+    <t>C3S2A334</t>
+  </si>
+  <si>
+    <t>C3S20132</t>
   </si>
 </sst>
 </file>
@@ -3378,7 +3387,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3421,6 +3430,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3434,7 +3449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3463,6 +3478,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3536,22 +3554,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R257" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="A1:R257" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R265" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="A1:R265" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}">
     <filterColumn colId="1">
       <filters>
-        <filter val="PST"/>
+        <filter val="MPTI"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="METODOLOGIA Y DISEÑO DE LA INVESTIGACION"/>
+        <filter val="TALLER DE TESIS I"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:R248">
-    <sortCondition ref="G2:G248"/>
-    <sortCondition ref="C2:C248"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A59:R61">
+    <sortCondition ref="E1:E257"/>
   </sortState>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{44E3F106-9108-4465-9FAD-59684B124153}" name="ciclo" dataDxfId="16"/>
@@ -3851,10 +3868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R257"/>
+  <dimension ref="A1:R265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A257" sqref="A257"/>
+      <selection activeCell="D267" sqref="D267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6856,19 +6873,19 @@
         <v>105</v>
       </c>
       <c r="E59" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>21</v>
@@ -6907,19 +6924,19 @@
         <v>105</v>
       </c>
       <c r="E60" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>21</v>
@@ -6958,19 +6975,19 @@
         <v>105</v>
       </c>
       <c r="E61" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>21</v>
@@ -14771,7 +14788,7 @@
       <c r="Q213" s="1"/>
       <c r="R213" s="1"/>
     </row>
-    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>1</v>
       </c>
@@ -14822,7 +14839,7 @@
       <c r="Q214" s="1"/>
       <c r="R214" s="1"/>
     </row>
-    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>1</v>
       </c>
@@ -15689,7 +15706,7 @@
       <c r="Q231" s="1"/>
       <c r="R231" s="1"/>
     </row>
-    <row r="232" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>1</v>
       </c>
@@ -15740,7 +15757,7 @@
       <c r="Q232" s="1"/>
       <c r="R232" s="1"/>
     </row>
-    <row r="233" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>1</v>
       </c>
@@ -17018,7 +17035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="257" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="10">
         <v>1</v>
       </c>
@@ -17072,6 +17089,462 @@
         <v>1</v>
       </c>
       <c r="R257" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="258" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="4">
+        <v>3</v>
+      </c>
+      <c r="B258" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C258" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D258" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E258" s="4">
+        <v>2</v>
+      </c>
+      <c r="F258" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="G258" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="H258" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="I258" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="J258" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K258" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L258" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M258" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N258" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O258" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P258" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q258" s="4">
+        <v>2</v>
+      </c>
+      <c r="R258" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="259" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A259" s="4">
+        <v>3</v>
+      </c>
+      <c r="B259" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C259" s="4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D259" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E259" s="4">
+        <v>2</v>
+      </c>
+      <c r="F259" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="G259" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="H259" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="I259" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="J259" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K259" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L259" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M259" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N259" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O259" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P259" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q259" s="4">
+        <v>2</v>
+      </c>
+      <c r="R259" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="260" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A260" s="3">
+        <v>3</v>
+      </c>
+      <c r="B260" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C260" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D260" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E260" s="3">
+        <v>3</v>
+      </c>
+      <c r="F260" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G260" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H260" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="I260" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="J260" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K260" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L260" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M260" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N260" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O260" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P260" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q260" s="3">
+        <v>3</v>
+      </c>
+      <c r="R260" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="261" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A261" s="3">
+        <v>3</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D261" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E261" s="3">
+        <v>3</v>
+      </c>
+      <c r="F261" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G261" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H261" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="I261" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="J261" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K261" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L261" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M261" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N261" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O261" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P261" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q261" s="3">
+        <v>3</v>
+      </c>
+      <c r="R261" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="262" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A262" s="12">
+        <v>3</v>
+      </c>
+      <c r="B262" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C262" s="12" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D262" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E262" s="12">
+        <v>1</v>
+      </c>
+      <c r="F262" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="G262" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="H262" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="I262" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="J262" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K262" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L262" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M262" s="12" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N262" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O262" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P262" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q262" s="12">
+        <v>1</v>
+      </c>
+      <c r="R262" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="263" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A263" s="12">
+        <v>3</v>
+      </c>
+      <c r="B263" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C263" s="12" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D263" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E263" s="12">
+        <v>1</v>
+      </c>
+      <c r="F263" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="G263" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="H263" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="I263" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="J263" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K263" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L263" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M263" s="12" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N263" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O263" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P263" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q263" s="12">
+        <v>1</v>
+      </c>
+      <c r="R263" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="264" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A264" s="5">
+        <v>3</v>
+      </c>
+      <c r="B264" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D264" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E264" s="5">
+        <v>2</v>
+      </c>
+      <c r="F264" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="G264" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="H264" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I264" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="J264" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="K264" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="L264" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="M264" s="5" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N264" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O264" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P264" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q264" s="5">
+        <v>2</v>
+      </c>
+      <c r="R264" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="265" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A265" s="12">
+        <v>1</v>
+      </c>
+      <c r="B265" s="12" t="s">
+        <v>959</v>
+      </c>
+      <c r="C265" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D265" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E265" s="12">
+        <v>2</v>
+      </c>
+      <c r="F265" s="12" t="s">
+        <v>961</v>
+      </c>
+      <c r="G265" s="12" t="s">
+        <v>962</v>
+      </c>
+      <c r="H265" s="12" t="s">
+        <v>963</v>
+      </c>
+      <c r="I265" s="12" t="s">
+        <v>964</v>
+      </c>
+      <c r="J265" s="12" t="s">
+        <v>808</v>
+      </c>
+      <c r="K265" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L265" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M265" s="12" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N265" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O265" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P265" s="12" t="s">
+        <v>960</v>
+      </c>
+      <c r="Q265" s="12">
+        <v>2</v>
+      </c>
+      <c r="R265" s="12" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on unmatched enrollements
</commit_message>
<xml_diff>
--- a/data/horarios/all.processed.xlsx
+++ b/data/horarios/all.processed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A986BBB9-0017-44BA-8ED9-95AAF354415B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57500973-D47B-4C8A-ABCB-C4AB68EAD420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="1142">
   <si>
     <t>ciclo</t>
   </si>
@@ -3375,6 +3375,90 @@
   </si>
   <si>
     <t>C2010201</t>
+  </si>
+  <si>
+    <t>C2010231</t>
+  </si>
+  <si>
+    <t>C3S10151</t>
+  </si>
+  <si>
+    <t>C202A242</t>
+  </si>
+  <si>
+    <t>C3P21234</t>
+  </si>
+  <si>
+    <t>C2020343</t>
+  </si>
+  <si>
+    <t>C2020344</t>
+  </si>
+  <si>
+    <t>C3P20131</t>
+  </si>
+  <si>
+    <t>C3P20133</t>
+  </si>
+  <si>
+    <t>C3P20134</t>
+  </si>
+  <si>
+    <t>C3P20111</t>
+  </si>
+  <si>
+    <t>C3P20531</t>
+  </si>
+  <si>
+    <t>C3P20532</t>
+  </si>
+  <si>
+    <t>C3P20533</t>
+  </si>
+  <si>
+    <t>C3P20534</t>
+  </si>
+  <si>
+    <t>C3P22233</t>
+  </si>
+  <si>
+    <t>C2020303</t>
+  </si>
+  <si>
+    <t>C2020341</t>
+  </si>
+  <si>
+    <t>C2020342</t>
+  </si>
+  <si>
+    <t>C3P20511</t>
+  </si>
+  <si>
+    <t>C3P20522</t>
+  </si>
+  <si>
+    <t>C3P20524</t>
+  </si>
+  <si>
+    <t>C3P205A4</t>
+  </si>
+  <si>
+    <t>C3P20512</t>
+  </si>
+  <si>
+    <t>C3P21431</t>
+  </si>
+  <si>
+    <t>C3P21432</t>
+  </si>
+  <si>
+    <t>C3S21113</t>
+  </si>
+  <si>
+    <t>C3S21112</t>
+  </si>
+  <si>
+    <t>C3S21111</t>
   </si>
 </sst>
 </file>
@@ -3390,7 +3474,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3439,6 +3523,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3452,7 +3572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3509,6 +3629,42 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3585,11 +3741,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R274" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="A1:R274" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}">
-    <filterColumn colId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R304" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="A1:R304" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}">
+    <filterColumn colId="3">
       <filters>
-        <filter val="DOMINGO"/>
+        <filter val="FUNDAMENTOS DE AUDITORIA TRIBUTARIA"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3894,10 +4050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R274"/>
+  <dimension ref="A1:R304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+      <selection activeCell="C309" sqref="C309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4744,55 +4900,55 @@
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+      <c r="A17" s="3">
         <v>3</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="15" t="s">
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M17" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="M17" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
     </row>
     <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
@@ -5356,55 +5512,55 @@
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+      <c r="A29" s="4">
         <v>3</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="15" t="s">
+      <c r="E29" s="4">
+        <v>1</v>
+      </c>
+      <c r="F29" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I29" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="K29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="L29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M29" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
+      <c r="M29" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
     </row>
     <row r="30" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -5611,55 +5767,55 @@
       <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+      <c r="A34" s="6">
         <v>4</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E34" s="1">
-        <v>1</v>
-      </c>
-      <c r="F34" s="15" t="s">
+      <c r="E34" s="6">
+        <v>1</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H34" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="I34" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="J34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="K34" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="L34" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M34" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N34" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
+      <c r="M34" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
     </row>
     <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
@@ -6069,56 +6225,56 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>1</v>
-      </c>
-      <c r="B43" s="1" t="s">
+    <row r="43" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+      <c r="A43" s="12">
+        <v>1</v>
+      </c>
+      <c r="B43" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="E43" s="1">
-        <v>1</v>
-      </c>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+      <c r="F43" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H43" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I43" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J43" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="K43" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="L43" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="M43" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N43" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
+      <c r="M43" s="12" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O43" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P43" s="12"/>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="12"/>
     </row>
     <row r="44" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
@@ -6325,55 +6481,55 @@
       <c r="R47" s="1"/>
     </row>
     <row r="48" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>1</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="A48" s="10">
+        <v>1</v>
+      </c>
+      <c r="B48" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="E48" s="1">
-        <v>1</v>
-      </c>
-      <c r="F48" s="15" t="s">
+      <c r="E48" s="10">
+        <v>1</v>
+      </c>
+      <c r="F48" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G48" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="I48" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="J48" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="K48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="L48" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M48" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N48" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
+      <c r="M48" s="10" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N48" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
     </row>
     <row r="49" spans="1:18" ht="66" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
@@ -6631,55 +6787,55 @@
       <c r="R53" s="1"/>
     </row>
     <row r="54" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>1</v>
-      </c>
-      <c r="B54" s="1" t="s">
+      <c r="A54" s="4">
+        <v>1</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="E54" s="1">
-        <v>1</v>
-      </c>
-      <c r="F54" s="15" t="s">
+      <c r="E54" s="4">
+        <v>1</v>
+      </c>
+      <c r="F54" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="G54" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="I54" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="J54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="K54" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="L54" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M54" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N54" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
+      <c r="M54" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N54" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
     </row>
     <row r="55" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
@@ -7249,55 +7405,55 @@
       <c r="R65" s="1"/>
     </row>
     <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>1</v>
-      </c>
-      <c r="B66" s="1" t="s">
+      <c r="A66" s="12">
+        <v>1</v>
+      </c>
+      <c r="B66" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="E66" s="1">
-        <v>1</v>
-      </c>
-      <c r="F66" s="15" t="s">
+      <c r="E66" s="12">
+        <v>1</v>
+      </c>
+      <c r="F66" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="G66" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="H66" s="1" t="s">
+      <c r="H66" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="I66" s="1" t="s">
+      <c r="I66" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="J66" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="K66" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="L66" s="1" t="s">
+      <c r="L66" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="M66" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N66" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O66" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
+      <c r="M66" s="12" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N66" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O66" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P66" s="12"/>
+      <c r="Q66" s="12"/>
+      <c r="R66" s="12"/>
     </row>
     <row r="67" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
@@ -7402,55 +7558,55 @@
       <c r="R68" s="1"/>
     </row>
     <row r="69" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
-        <v>1</v>
-      </c>
-      <c r="B69" s="1" t="s">
+      <c r="A69" s="4">
+        <v>1</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="E69" s="1">
-        <v>1</v>
-      </c>
-      <c r="F69" s="15" t="s">
+      <c r="E69" s="4">
+        <v>1</v>
+      </c>
+      <c r="F69" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="G69" s="1" t="s">
+      <c r="G69" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="H69" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="I69" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="J69" s="1" t="s">
+      <c r="J69" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="K69" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="L69" s="1" t="s">
+      <c r="L69" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="M69" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N69" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O69" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
+      <c r="M69" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N69" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O69" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="4"/>
     </row>
     <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
@@ -7657,259 +7813,259 @@
       <c r="R73" s="1"/>
     </row>
     <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
+      <c r="A74" s="6">
         <v>3</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E74" s="1">
-        <v>1</v>
-      </c>
-      <c r="F74" s="15" t="s">
+      <c r="E74" s="6">
+        <v>1</v>
+      </c>
+      <c r="F74" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="G74" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="H74" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="I74" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="J74" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="K74" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="L74" s="1" t="s">
+      <c r="L74" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="M74" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N74" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O74" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
+      <c r="M74" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N74" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O74" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P74" s="6"/>
+      <c r="Q74" s="6"/>
+      <c r="R74" s="6"/>
     </row>
     <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1">
+      <c r="A75" s="5">
         <v>3</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="5">
         <v>2</v>
       </c>
-      <c r="F75" s="15" t="s">
+      <c r="F75" s="19" t="s">
         <v>377</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="G75" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="H75" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I75" s="1" t="s">
+      <c r="I75" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="J75" s="1" t="s">
+      <c r="J75" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="K75" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="L75" s="1" t="s">
+      <c r="L75" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M75" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N75" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O75" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
+      <c r="M75" s="5" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N75" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O75" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P75" s="5"/>
+      <c r="Q75" s="5"/>
+      <c r="R75" s="5"/>
     </row>
     <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
+      <c r="A76" s="3">
         <v>3</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E76" s="1">
-        <v>1</v>
-      </c>
-      <c r="F76" s="15" t="s">
+      <c r="E76" s="3">
+        <v>1</v>
+      </c>
+      <c r="F76" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="G76" s="1" t="s">
+      <c r="G76" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="H76" s="1" t="s">
+      <c r="H76" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="I76" s="1" t="s">
+      <c r="I76" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="J76" s="1" t="s">
+      <c r="J76" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="K76" s="1" t="s">
+      <c r="K76" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="L76" s="1" t="s">
+      <c r="L76" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="M76" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N76" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O76" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
+      <c r="M76" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N76" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O76" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3"/>
     </row>
     <row r="77" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
+      <c r="A77" s="4">
         <v>3</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="E77" s="1">
-        <v>1</v>
-      </c>
-      <c r="F77" s="15" t="s">
+      <c r="E77" s="4">
+        <v>1</v>
+      </c>
+      <c r="F77" s="18" t="s">
         <v>388</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="G77" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="H77" s="1" t="s">
+      <c r="H77" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="I77" s="1" t="s">
+      <c r="I77" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="J77" s="1" t="s">
+      <c r="J77" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="K77" s="1" t="s">
+      <c r="K77" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="L77" s="1" t="s">
+      <c r="L77" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="M77" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N77" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O77" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
+      <c r="M77" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N77" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O77" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
     </row>
     <row r="78" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
+      <c r="A78" s="10">
         <v>3</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="E78" s="1">
-        <v>1</v>
-      </c>
-      <c r="F78" s="15" t="s">
+      <c r="E78" s="10">
+        <v>1</v>
+      </c>
+      <c r="F78" s="20" t="s">
         <v>348</v>
       </c>
-      <c r="G78" s="1" t="s">
+      <c r="G78" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="H78" s="1" t="s">
+      <c r="H78" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="I78" s="1" t="s">
+      <c r="I78" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="J78" s="1" t="s">
+      <c r="J78" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="K78" s="1" t="s">
+      <c r="K78" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="L78" s="1" t="s">
+      <c r="L78" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="M78" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N78" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O78" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P78" s="1"/>
-      <c r="Q78" s="1"/>
-      <c r="R78" s="1"/>
+      <c r="M78" s="10" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N78" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O78" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P78" s="10"/>
+      <c r="Q78" s="10"/>
+      <c r="R78" s="10"/>
     </row>
     <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
@@ -7963,157 +8119,157 @@
       <c r="R79" s="1"/>
     </row>
     <row r="80" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
+      <c r="A80" s="3">
         <v>4</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="E80" s="1">
-        <v>1</v>
-      </c>
-      <c r="F80" s="15" t="s">
+      <c r="E80" s="3">
+        <v>1</v>
+      </c>
+      <c r="F80" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="G80" s="1" t="s">
+      <c r="G80" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="H80" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="I80" s="1" t="s">
+      <c r="I80" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="J80" s="1" t="s">
+      <c r="J80" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="K80" s="1" t="s">
+      <c r="K80" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="L80" s="1" t="s">
+      <c r="L80" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="M80" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N80" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O80" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P80" s="1"/>
-      <c r="Q80" s="1"/>
-      <c r="R80" s="1"/>
+      <c r="M80" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N80" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O80" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P80" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
     </row>
     <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1">
+      <c r="A81" s="4">
         <v>4</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="E81" s="1">
-        <v>1</v>
-      </c>
-      <c r="F81" s="15" t="s">
+      <c r="E81" s="4">
+        <v>1</v>
+      </c>
+      <c r="F81" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="G81" s="1" t="s">
+      <c r="G81" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="H81" s="1" t="s">
+      <c r="H81" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="I81" s="1" t="s">
+      <c r="I81" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="J81" s="1" t="s">
+      <c r="J81" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="K81" s="1" t="s">
+      <c r="K81" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="L81" s="1" t="s">
+      <c r="L81" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="M81" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N81" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O81" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P81" s="1"/>
-      <c r="Q81" s="1"/>
-      <c r="R81" s="1"/>
+      <c r="M81" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N81" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O81" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="4"/>
     </row>
     <row r="82" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
+      <c r="A82" s="6">
         <v>4</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D82" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="E82" s="1">
-        <v>1</v>
-      </c>
-      <c r="F82" s="15" t="s">
+      <c r="E82" s="6">
+        <v>1</v>
+      </c>
+      <c r="F82" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="G82" s="1" t="s">
+      <c r="G82" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="H82" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="I82" s="1" t="s">
+      <c r="I82" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="J82" s="1" t="s">
+      <c r="J82" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="K82" s="1" t="s">
+      <c r="K82" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="L82" s="1" t="s">
+      <c r="L82" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="M82" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N82" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O82" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P82" s="1"/>
-      <c r="Q82" s="1"/>
-      <c r="R82" s="1"/>
+      <c r="M82" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N82" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O82" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P82" s="6"/>
+      <c r="Q82" s="6"/>
+      <c r="R82" s="6"/>
     </row>
     <row r="83" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
@@ -9187,106 +9343,106 @@
       <c r="R103" s="1"/>
     </row>
     <row r="104" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="1">
-        <v>1</v>
-      </c>
-      <c r="B104" s="1" t="s">
+      <c r="A104" s="4">
+        <v>1</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="E104" s="1">
-        <v>1</v>
-      </c>
-      <c r="F104" s="15" t="s">
+      <c r="E104" s="4">
+        <v>1</v>
+      </c>
+      <c r="F104" s="18" t="s">
         <v>513</v>
       </c>
-      <c r="G104" s="1" t="s">
+      <c r="G104" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="H104" s="1" t="s">
+      <c r="H104" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="I104" s="1" t="s">
+      <c r="I104" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J104" s="1" t="s">
+      <c r="J104" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="K104" s="1" t="s">
+      <c r="K104" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="L104" s="1" t="s">
+      <c r="L104" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="M104" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N104" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O104" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P104" s="1"/>
-      <c r="Q104" s="1"/>
-      <c r="R104" s="1"/>
+      <c r="M104" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N104" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O104" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="4"/>
+      <c r="R104" s="4"/>
     </row>
     <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="1">
-        <v>1</v>
-      </c>
-      <c r="B105" s="1" t="s">
+      <c r="A105" s="6">
+        <v>1</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="6" t="s">
         <v>515</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D105" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="E105" s="1">
-        <v>1</v>
-      </c>
-      <c r="F105" s="15" t="s">
+      <c r="E105" s="6">
+        <v>1</v>
+      </c>
+      <c r="F105" s="13" t="s">
         <v>517</v>
       </c>
-      <c r="G105" s="1" t="s">
+      <c r="G105" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="H105" s="1" t="s">
+      <c r="H105" s="6" t="s">
         <v>518</v>
       </c>
-      <c r="I105" s="1" t="s">
+      <c r="I105" s="6" t="s">
         <v>519</v>
       </c>
-      <c r="J105" s="1" t="s">
+      <c r="J105" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="K105" s="1" t="s">
+      <c r="K105" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="L105" s="1" t="s">
+      <c r="L105" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="M105" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N105" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O105" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P105" s="1"/>
-      <c r="Q105" s="1"/>
-      <c r="R105" s="1"/>
+      <c r="M105" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N105" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O105" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P105" s="6"/>
+      <c r="Q105" s="6"/>
+      <c r="R105" s="6"/>
     </row>
     <row r="106" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
@@ -9340,55 +9496,55 @@
       <c r="R106" s="1"/>
     </row>
     <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="1">
+      <c r="A107" s="6">
         <v>2</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D107" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E107" s="1">
-        <v>1</v>
-      </c>
-      <c r="F107" s="15" t="s">
+      <c r="E107" s="6">
+        <v>1</v>
+      </c>
+      <c r="F107" s="13" t="s">
         <v>525</v>
       </c>
-      <c r="G107" s="1" t="s">
+      <c r="G107" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="H107" s="1" t="s">
+      <c r="H107" s="6" t="s">
         <v>527</v>
       </c>
-      <c r="I107" s="1" t="s">
+      <c r="I107" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="J107" s="1" t="s">
+      <c r="J107" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="K107" s="1" t="s">
+      <c r="K107" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="L107" s="1" t="s">
+      <c r="L107" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="M107" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N107" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O107" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P107" s="1"/>
-      <c r="Q107" s="1"/>
-      <c r="R107" s="1"/>
+      <c r="M107" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N107" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O107" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P107" s="6"/>
+      <c r="Q107" s="6"/>
+      <c r="R107" s="6"/>
     </row>
     <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
@@ -9544,361 +9700,361 @@
       <c r="R110" s="1"/>
     </row>
     <row r="111" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="1">
+      <c r="A111" s="5">
         <v>2</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="5" t="s">
         <v>500</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D111" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="E111" s="1">
-        <v>1</v>
-      </c>
-      <c r="F111" s="15" t="s">
+      <c r="E111" s="5">
+        <v>1</v>
+      </c>
+      <c r="F111" s="19" t="s">
         <v>540</v>
       </c>
-      <c r="G111" s="1" t="s">
+      <c r="G111" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="H111" s="1" t="s">
+      <c r="H111" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="I111" s="1" t="s">
+      <c r="I111" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="J111" s="1" t="s">
+      <c r="J111" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="K111" s="1" t="s">
+      <c r="K111" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="L111" s="1" t="s">
+      <c r="L111" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M111" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N111" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O111" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P111" s="1"/>
-      <c r="Q111" s="1"/>
-      <c r="R111" s="1"/>
+      <c r="M111" s="5" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N111" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O111" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P111" s="5"/>
+      <c r="Q111" s="5"/>
+      <c r="R111" s="5"/>
     </row>
     <row r="112" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="1">
+      <c r="A112" s="5">
         <v>2</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="5" t="s">
         <v>500</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="E112" s="1">
-        <v>1</v>
-      </c>
-      <c r="F112" s="15" t="s">
+      <c r="E112" s="5">
+        <v>1</v>
+      </c>
+      <c r="F112" s="19" t="s">
         <v>517</v>
       </c>
-      <c r="G112" s="1" t="s">
+      <c r="G112" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H112" s="1" t="s">
+      <c r="H112" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="I112" s="1" t="s">
+      <c r="I112" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="J112" s="1" t="s">
+      <c r="J112" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="K112" s="1" t="s">
+      <c r="K112" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="L112" s="1" t="s">
+      <c r="L112" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M112" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N112" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O112" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P112" s="1"/>
-      <c r="Q112" s="1"/>
-      <c r="R112" s="1"/>
+      <c r="M112" s="5" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N112" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O112" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P112" s="5"/>
+      <c r="Q112" s="5"/>
+      <c r="R112" s="5"/>
     </row>
     <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="1">
+      <c r="A113" s="12">
         <v>3</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="12" t="s">
         <v>500</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="12" t="s">
         <v>546</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D113" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E113" s="1">
-        <v>1</v>
-      </c>
-      <c r="F113" s="15" t="s">
+      <c r="E113" s="12">
+        <v>1</v>
+      </c>
+      <c r="F113" s="21" t="s">
         <v>547</v>
       </c>
-      <c r="G113" s="1" t="s">
+      <c r="G113" s="12" t="s">
         <v>548</v>
       </c>
-      <c r="H113" s="1" t="s">
+      <c r="H113" s="12" t="s">
         <v>549</v>
       </c>
-      <c r="I113" s="1" t="s">
+      <c r="I113" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="J113" s="1" t="s">
+      <c r="J113" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="K113" s="1" t="s">
+      <c r="K113" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="L113" s="1" t="s">
+      <c r="L113" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="M113" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N113" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O113" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P113" s="1"/>
-      <c r="Q113" s="1"/>
-      <c r="R113" s="1"/>
+      <c r="M113" s="12" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N113" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O113" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P113" s="12"/>
+      <c r="Q113" s="12"/>
+      <c r="R113" s="12"/>
     </row>
     <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="1">
+      <c r="A114" s="12">
         <v>3</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="12" t="s">
         <v>500</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="12" t="s">
         <v>546</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D114" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E114" s="1">
+      <c r="E114" s="12">
         <v>2</v>
       </c>
-      <c r="F114" s="15" t="s">
+      <c r="F114" s="21" t="s">
         <v>551</v>
       </c>
-      <c r="G114" s="1" t="s">
+      <c r="G114" s="12" t="s">
         <v>552</v>
       </c>
-      <c r="H114" s="1" t="s">
+      <c r="H114" s="12" t="s">
         <v>417</v>
       </c>
-      <c r="I114" s="1" t="s">
+      <c r="I114" s="12" t="s">
         <v>553</v>
       </c>
-      <c r="J114" s="1" t="s">
+      <c r="J114" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="K114" s="1" t="s">
+      <c r="K114" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="L114" s="1" t="s">
+      <c r="L114" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="M114" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N114" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O114" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P114" s="1"/>
-      <c r="Q114" s="1"/>
-      <c r="R114" s="1"/>
+      <c r="M114" s="12" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N114" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O114" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P114" s="12"/>
+      <c r="Q114" s="12"/>
+      <c r="R114" s="12"/>
     </row>
     <row r="115" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="1">
+      <c r="A115" s="5">
         <v>3</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="5" t="s">
         <v>500</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D115" s="5" t="s">
         <v>555</v>
       </c>
-      <c r="E115" s="1">
-        <v>1</v>
-      </c>
-      <c r="F115" s="15" t="s">
+      <c r="E115" s="5">
+        <v>1</v>
+      </c>
+      <c r="F115" s="19" t="s">
         <v>513</v>
       </c>
-      <c r="G115" s="1" t="s">
+      <c r="G115" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="H115" s="1" t="s">
+      <c r="H115" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="I115" s="1" t="s">
+      <c r="I115" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J115" s="1" t="s">
+      <c r="J115" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="K115" s="1" t="s">
+      <c r="K115" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="L115" s="1" t="s">
+      <c r="L115" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="M115" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N115" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O115" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P115" s="1"/>
-      <c r="Q115" s="1"/>
-      <c r="R115" s="1"/>
+      <c r="M115" s="5" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N115" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O115" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P115" s="5"/>
+      <c r="Q115" s="5"/>
+      <c r="R115" s="5"/>
     </row>
     <row r="116" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="1">
+      <c r="A116" s="6">
         <v>3</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="6" t="s">
         <v>556</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D116" s="6" t="s">
         <v>557</v>
       </c>
-      <c r="E116" s="1">
-        <v>1</v>
-      </c>
-      <c r="F116" s="15" t="s">
+      <c r="E116" s="6">
+        <v>1</v>
+      </c>
+      <c r="F116" s="13" t="s">
         <v>558</v>
       </c>
-      <c r="G116" s="1" t="s">
+      <c r="G116" s="6" t="s">
         <v>559</v>
       </c>
-      <c r="H116" s="1" t="s">
+      <c r="H116" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="I116" s="1" t="s">
+      <c r="I116" s="6" t="s">
         <v>560</v>
       </c>
-      <c r="J116" s="1" t="s">
+      <c r="J116" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="K116" s="1" t="s">
+      <c r="K116" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="L116" s="1" t="s">
+      <c r="L116" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="M116" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N116" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O116" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P116" s="1"/>
-      <c r="Q116" s="1"/>
-      <c r="R116" s="1"/>
+      <c r="M116" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N116" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O116" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P116" s="6"/>
+      <c r="Q116" s="6"/>
+      <c r="R116" s="6"/>
     </row>
     <row r="117" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="1">
+      <c r="A117" s="3">
         <v>3</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D117" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="E117" s="1">
-        <v>1</v>
-      </c>
-      <c r="F117" s="15" t="s">
+      <c r="E117" s="3">
+        <v>1</v>
+      </c>
+      <c r="F117" s="16" t="s">
         <v>521</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="G117" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="H117" s="1" t="s">
+      <c r="H117" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="I117" s="1" t="s">
+      <c r="I117" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="J117" s="1" t="s">
+      <c r="J117" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="K117" s="1" t="s">
+      <c r="K117" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="L117" s="1" t="s">
+      <c r="L117" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="M117" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N117" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O117" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P117" s="1"/>
-      <c r="Q117" s="1"/>
-      <c r="R117" s="1"/>
+      <c r="M117" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N117" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O117" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P117" s="3"/>
+      <c r="Q117" s="3"/>
+      <c r="R117" s="3"/>
     </row>
     <row r="118" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
@@ -10621,106 +10777,106 @@
       <c r="R131" s="1"/>
     </row>
     <row r="132" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="1">
+      <c r="A132" s="10">
         <v>3</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="C132" s="10" t="s">
         <v>611</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D132" s="10" t="s">
         <v>612</v>
       </c>
-      <c r="E132" s="1">
-        <v>1</v>
-      </c>
-      <c r="F132" s="15" t="s">
+      <c r="E132" s="10">
+        <v>1</v>
+      </c>
+      <c r="F132" s="20" t="s">
         <v>613</v>
       </c>
-      <c r="G132" s="1" t="s">
+      <c r="G132" s="10" t="s">
         <v>614</v>
       </c>
-      <c r="H132" s="1" t="s">
+      <c r="H132" s="10" t="s">
         <v>615</v>
       </c>
-      <c r="I132" s="1" t="s">
+      <c r="I132" s="10" t="s">
         <v>616</v>
       </c>
-      <c r="J132" s="1" t="s">
+      <c r="J132" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="K132" s="1" t="s">
+      <c r="K132" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="L132" s="1" t="s">
+      <c r="L132" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="M132" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N132" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O132" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P132" s="1"/>
-      <c r="Q132" s="1"/>
-      <c r="R132" s="1"/>
+      <c r="M132" s="10" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N132" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O132" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="10"/>
+      <c r="R132" s="10"/>
     </row>
     <row r="133" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="1">
+      <c r="A133" s="4">
         <v>3</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="C133" s="4" t="s">
         <v>617</v>
       </c>
-      <c r="D133" s="1" t="s">
+      <c r="D133" s="4" t="s">
         <v>618</v>
       </c>
-      <c r="E133" s="1">
-        <v>1</v>
-      </c>
-      <c r="F133" s="15" t="s">
+      <c r="E133" s="4">
+        <v>1</v>
+      </c>
+      <c r="F133" s="18" t="s">
         <v>619</v>
       </c>
-      <c r="G133" s="1" t="s">
+      <c r="G133" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="H133" s="1" t="s">
+      <c r="H133" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="I133" s="1" t="s">
+      <c r="I133" s="4" t="s">
         <v>621</v>
       </c>
-      <c r="J133" s="1" t="s">
+      <c r="J133" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="K133" s="1" t="s">
+      <c r="K133" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="L133" s="1" t="s">
+      <c r="L133" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="M133" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N133" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O133" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P133" s="1"/>
-      <c r="Q133" s="1"/>
-      <c r="R133" s="1"/>
+      <c r="M133" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N133" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O133" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P133" s="4"/>
+      <c r="Q133" s="4"/>
+      <c r="R133" s="4"/>
     </row>
     <row r="134" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
@@ -11232,7 +11388,7 @@
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="5">
         <v>1</v>
       </c>
@@ -12611,7 +12767,7 @@
         <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
         <v>1</v>
       </c>
-      <c r="N170" s="1" t="b">
+      <c r="N170" s="6" t="b">
         <v>0</v>
       </c>
       <c r="O170" s="6" t="s">
@@ -13341,7 +13497,7 @@
       <c r="Q184" s="1"/>
       <c r="R184" s="1"/>
     </row>
-    <row r="185" spans="1:18" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:18" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>1</v>
       </c>
@@ -13392,7 +13548,7 @@
       <c r="Q185" s="1"/>
       <c r="R185" s="1"/>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>2</v>
       </c>
@@ -13545,7 +13701,7 @@
       <c r="Q188" s="1"/>
       <c r="R188" s="1"/>
     </row>
-    <row r="189" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>2</v>
       </c>
@@ -13698,7 +13854,7 @@
       <c r="Q191" s="1"/>
       <c r="R191" s="1"/>
     </row>
-    <row r="192" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>1</v>
       </c>
@@ -13953,7 +14109,7 @@
       <c r="Q196" s="1"/>
       <c r="R196" s="1"/>
     </row>
-    <row r="197" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>2</v>
       </c>
@@ -14004,7 +14160,7 @@
       <c r="Q197" s="1"/>
       <c r="R197" s="1"/>
     </row>
-    <row r="198" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>2</v>
       </c>
@@ -14259,7 +14415,7 @@
       <c r="Q202" s="1"/>
       <c r="R202" s="1"/>
     </row>
-    <row r="203" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>1</v>
       </c>
@@ -14310,7 +14466,7 @@
       <c r="Q203" s="1"/>
       <c r="R203" s="1"/>
     </row>
-    <row r="204" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>1</v>
       </c>
@@ -14514,7 +14670,7 @@
       <c r="Q207" s="1"/>
       <c r="R207" s="1"/>
     </row>
-    <row r="208" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>2</v>
       </c>
@@ -14565,7 +14721,7 @@
       <c r="Q208" s="1"/>
       <c r="R208" s="1"/>
     </row>
-    <row r="209" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>2</v>
       </c>
@@ -14820,7 +14976,7 @@
       <c r="Q213" s="1"/>
       <c r="R213" s="1"/>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="5">
         <v>1</v>
       </c>
@@ -14877,7 +15033,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>1</v>
       </c>
@@ -14928,7 +15084,7 @@
       <c r="Q215" s="1"/>
       <c r="R215" s="1"/>
     </row>
-    <row r="216" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>1</v>
       </c>
@@ -15183,7 +15339,7 @@
       <c r="Q220" s="1"/>
       <c r="R220" s="1"/>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>2</v>
       </c>
@@ -15234,7 +15390,7 @@
       <c r="Q221" s="1"/>
       <c r="R221" s="1"/>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>2</v>
       </c>
@@ -15285,7 +15441,7 @@
       <c r="Q222" s="1"/>
       <c r="R222" s="1"/>
     </row>
-    <row r="223" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>2</v>
       </c>
@@ -17473,63 +17629,63 @@
       </c>
     </row>
     <row r="264" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A264" s="5">
+      <c r="A264" s="32">
         <v>3</v>
       </c>
-      <c r="B264" s="5" t="s">
+      <c r="B264" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="C264" s="5" t="s">
+      <c r="C264" s="32" t="s">
         <v>1106</v>
       </c>
-      <c r="D264" s="5" t="s">
+      <c r="D264" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="E264" s="5">
+      <c r="E264" s="32">
         <v>2</v>
       </c>
-      <c r="F264" s="19" t="s">
+      <c r="F264" s="33" t="s">
         <v>377</v>
       </c>
-      <c r="G264" s="5" t="s">
+      <c r="G264" s="32" t="s">
         <v>378</v>
       </c>
-      <c r="H264" s="5" t="s">
+      <c r="H264" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="I264" s="5" t="s">
+      <c r="I264" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="J264" s="5" t="s">
+      <c r="J264" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="K264" s="5" t="s">
+      <c r="K264" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="L264" s="5" t="s">
+      <c r="L264" s="32" t="s">
         <v>323</v>
       </c>
-      <c r="M264" s="5" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>1</v>
-      </c>
-      <c r="N264" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O264" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P264" s="5" t="s">
+      <c r="M264" s="32" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N264" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O264" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P264" s="32" t="s">
         <v>373</v>
       </c>
-      <c r="Q264" s="5">
+      <c r="Q264" s="32">
         <v>2</v>
       </c>
-      <c r="R264" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="265" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R264" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="265" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="12">
         <v>1</v>
       </c>
@@ -17871,7 +18027,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="271" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="5">
         <v>1</v>
       </c>
@@ -17928,7 +18084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="272" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="5">
         <v>1</v>
       </c>
@@ -18096,6 +18252,1716 @@
         <v>1</v>
       </c>
       <c r="R274" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="275" spans="1:18" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A275" s="3">
+        <v>3</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="C275" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D275" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="E275" s="3">
+        <v>1</v>
+      </c>
+      <c r="F275" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="G275" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H275" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="I275" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="J275" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K275" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L275" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M275" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N275" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O275" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P275" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="Q275" s="3">
+        <v>1</v>
+      </c>
+      <c r="R275" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="276" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A276" s="6">
+        <v>6</v>
+      </c>
+      <c r="B276" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="C276" s="6" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D276" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E276" s="6">
+        <v>1</v>
+      </c>
+      <c r="F276" s="13" t="s">
+        <v>662</v>
+      </c>
+      <c r="G276" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="H276" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="I276" s="6" t="s">
+        <v>664</v>
+      </c>
+      <c r="J276" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K276" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L276" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="M276" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N276" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O276" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P276" s="6" t="s">
+        <v>661</v>
+      </c>
+      <c r="Q276" s="6">
+        <v>1</v>
+      </c>
+      <c r="R276" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="277" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A277" s="6">
+        <v>4</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C277" s="6" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D277" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E277" s="6">
+        <v>1</v>
+      </c>
+      <c r="F277" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G277" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="H277" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="I277" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="J277" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K277" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L277" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M277" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N277" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O277" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P277" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q277" s="6">
+        <v>1</v>
+      </c>
+      <c r="R277" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="278" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A278" s="22">
+        <v>3</v>
+      </c>
+      <c r="B278" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C278" s="22" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D278" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E278" s="22">
+        <v>1</v>
+      </c>
+      <c r="F278" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G278" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H278" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="I278" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="J278" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K278" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L278" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M278" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N278" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O278" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P278" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q278" s="22">
+        <v>1</v>
+      </c>
+      <c r="R278" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="279" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A279" s="24">
+        <v>3</v>
+      </c>
+      <c r="B279" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C279" s="24" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D279" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E279" s="24">
+        <v>1</v>
+      </c>
+      <c r="F279" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="G279" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H279" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="I279" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="J279" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K279" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L279" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M279" s="24" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N279" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O279" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P279" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q279" s="24">
+        <v>1</v>
+      </c>
+      <c r="R279" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="280" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A280" s="26">
+        <v>4</v>
+      </c>
+      <c r="B280" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="C280" s="26" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D280" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="E280" s="26">
+        <v>1</v>
+      </c>
+      <c r="F280" s="27" t="s">
+        <v>409</v>
+      </c>
+      <c r="G280" s="26" t="s">
+        <v>410</v>
+      </c>
+      <c r="H280" s="26" t="s">
+        <v>411</v>
+      </c>
+      <c r="I280" s="26" t="s">
+        <v>412</v>
+      </c>
+      <c r="J280" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="K280" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="L280" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="M280" s="26" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N280" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O280" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P280" s="26" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q280" s="26">
+        <v>1</v>
+      </c>
+      <c r="R280" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="281" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A281" s="24">
+        <v>3</v>
+      </c>
+      <c r="B281" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="C281" s="24" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D281" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="E281" s="24">
+        <v>1</v>
+      </c>
+      <c r="F281" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="G281" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="H281" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="I281" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="J281" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="K281" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="L281" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="M281" s="24" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N281" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O281" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P281" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q281" s="24">
+        <v>1</v>
+      </c>
+      <c r="R281" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="282" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A282" s="22">
+        <v>3</v>
+      </c>
+      <c r="B282" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="C282" s="22" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D282" s="22" t="s">
+        <v>387</v>
+      </c>
+      <c r="E282" s="22">
+        <v>1</v>
+      </c>
+      <c r="F282" s="23" t="s">
+        <v>388</v>
+      </c>
+      <c r="G282" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="H282" s="22" t="s">
+        <v>390</v>
+      </c>
+      <c r="I282" s="22" t="s">
+        <v>391</v>
+      </c>
+      <c r="J282" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="K282" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="L282" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="M282" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N282" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O282" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P282" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q282" s="22">
+        <v>1</v>
+      </c>
+      <c r="R282" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="283" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A283" s="28">
+        <v>3</v>
+      </c>
+      <c r="B283" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="C283" s="28" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D283" s="28" t="s">
+        <v>393</v>
+      </c>
+      <c r="E283" s="28">
+        <v>1</v>
+      </c>
+      <c r="F283" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G283" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="H283" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="I283" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="J283" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="K283" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="L283" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="M283" s="28" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N283" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O283" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P283" s="28" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q283" s="28">
+        <v>1</v>
+      </c>
+      <c r="R283" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="284" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A284" s="30">
+        <v>1</v>
+      </c>
+      <c r="B284" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="C284" s="30" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D284" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="E284" s="30">
+        <v>1</v>
+      </c>
+      <c r="F284" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="G284" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="H284" s="30" t="s">
+        <v>331</v>
+      </c>
+      <c r="I284" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="J284" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="K284" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="L284" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="M284" s="30" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N284" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O284" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="P284" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q284" s="30">
+        <v>1</v>
+      </c>
+      <c r="R284" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="285" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A285" s="26">
+        <v>3</v>
+      </c>
+      <c r="B285" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="C285" s="26" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D285" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E285" s="26">
+        <v>1</v>
+      </c>
+      <c r="F285" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="G285" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="H285" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="I285" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="J285" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="K285" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="L285" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="M285" s="26" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N285" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O285" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P285" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q285" s="26">
+        <v>1</v>
+      </c>
+      <c r="R285" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="286" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A286" s="32">
+        <v>3</v>
+      </c>
+      <c r="B286" s="32" t="s">
+        <v>500</v>
+      </c>
+      <c r="C286" s="32" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D286" s="32" t="s">
+        <v>555</v>
+      </c>
+      <c r="E286" s="32">
+        <v>1</v>
+      </c>
+      <c r="F286" s="33" t="s">
+        <v>513</v>
+      </c>
+      <c r="G286" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="H286" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="I286" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="J286" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="K286" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="L286" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="M286" s="32" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N286" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O286" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P286" s="32" t="s">
+        <v>554</v>
+      </c>
+      <c r="Q286" s="32">
+        <v>1</v>
+      </c>
+      <c r="R286" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="287" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A287" s="26">
+        <v>3</v>
+      </c>
+      <c r="B287" s="26" t="s">
+        <v>500</v>
+      </c>
+      <c r="C287" s="26" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D287" s="26" t="s">
+        <v>557</v>
+      </c>
+      <c r="E287" s="26">
+        <v>1</v>
+      </c>
+      <c r="F287" s="27" t="s">
+        <v>558</v>
+      </c>
+      <c r="G287" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="H287" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="I287" s="26" t="s">
+        <v>560</v>
+      </c>
+      <c r="J287" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="K287" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="L287" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="M287" s="26" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N287" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O287" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P287" s="26" t="s">
+        <v>556</v>
+      </c>
+      <c r="Q287" s="26">
+        <v>1</v>
+      </c>
+      <c r="R287" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="288" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A288" s="30">
+        <v>3</v>
+      </c>
+      <c r="B288" s="30" t="s">
+        <v>500</v>
+      </c>
+      <c r="C288" s="30" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D288" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E288" s="30">
+        <v>1</v>
+      </c>
+      <c r="F288" s="31" t="s">
+        <v>547</v>
+      </c>
+      <c r="G288" s="30" t="s">
+        <v>548</v>
+      </c>
+      <c r="H288" s="30" t="s">
+        <v>549</v>
+      </c>
+      <c r="I288" s="30" t="s">
+        <v>550</v>
+      </c>
+      <c r="J288" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="K288" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="L288" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="M288" s="30" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N288" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O288" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="P288" s="30" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q288" s="30">
+        <v>1</v>
+      </c>
+      <c r="R288" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="289" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="30">
+        <v>3</v>
+      </c>
+      <c r="B289" s="30" t="s">
+        <v>500</v>
+      </c>
+      <c r="C289" s="30" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D289" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E289" s="30">
+        <v>2</v>
+      </c>
+      <c r="F289" s="31" t="s">
+        <v>551</v>
+      </c>
+      <c r="G289" s="30" t="s">
+        <v>552</v>
+      </c>
+      <c r="H289" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="I289" s="30" t="s">
+        <v>553</v>
+      </c>
+      <c r="J289" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="K289" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="L289" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="M289" s="30" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N289" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O289" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="P289" s="30" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q289" s="30">
+        <v>2</v>
+      </c>
+      <c r="R289" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="290" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A290" s="24">
+        <v>3</v>
+      </c>
+      <c r="B290" s="24" t="s">
+        <v>500</v>
+      </c>
+      <c r="C290" s="24" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D290" s="24" t="s">
+        <v>562</v>
+      </c>
+      <c r="E290" s="24">
+        <v>1</v>
+      </c>
+      <c r="F290" s="25" t="s">
+        <v>521</v>
+      </c>
+      <c r="G290" s="24" t="s">
+        <v>371</v>
+      </c>
+      <c r="H290" s="24" t="s">
+        <v>522</v>
+      </c>
+      <c r="I290" s="24" t="s">
+        <v>523</v>
+      </c>
+      <c r="J290" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="K290" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="L290" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="M290" s="24" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N290" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O290" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P290" s="24" t="s">
+        <v>561</v>
+      </c>
+      <c r="Q290" s="24">
+        <v>1</v>
+      </c>
+      <c r="R290" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="291" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A291" s="24">
+        <v>3</v>
+      </c>
+      <c r="B291" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C291" s="24" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D291" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E291" s="24">
+        <v>1</v>
+      </c>
+      <c r="F291" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="G291" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H291" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="I291" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="J291" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K291" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L291" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M291" s="24" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N291" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O291" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P291" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q291" s="24">
+        <v>1</v>
+      </c>
+      <c r="R291" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="292" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A292" s="22">
+        <v>1</v>
+      </c>
+      <c r="B292" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="C292" s="22" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D292" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="E292" s="22">
+        <v>1</v>
+      </c>
+      <c r="F292" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="G292" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="H292" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="I292" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="J292" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="K292" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="L292" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="M292" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N292" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O292" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P292" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q292" s="22">
+        <v>1</v>
+      </c>
+      <c r="R292" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="293" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A293" s="24">
+        <v>4</v>
+      </c>
+      <c r="B293" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="C293" s="24" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D293" s="24" t="s">
+        <v>400</v>
+      </c>
+      <c r="E293" s="24">
+        <v>1</v>
+      </c>
+      <c r="F293" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="G293" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="H293" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="I293" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="J293" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="K293" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="L293" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="M293" s="24" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N293" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O293" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P293" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q293" s="24">
+        <v>1</v>
+      </c>
+      <c r="R293" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="294" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A294" s="22">
+        <v>4</v>
+      </c>
+      <c r="B294" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="C294" s="22" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D294" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="E294" s="22">
+        <v>1</v>
+      </c>
+      <c r="F294" s="23" t="s">
+        <v>403</v>
+      </c>
+      <c r="G294" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="H294" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="I294" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="J294" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="K294" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="L294" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="M294" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N294" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O294" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P294" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q294" s="22">
+        <v>1</v>
+      </c>
+      <c r="R294" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="295" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A295" s="22">
+        <v>1</v>
+      </c>
+      <c r="B295" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="C295" s="22" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D295" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="E295" s="22">
+        <v>1</v>
+      </c>
+      <c r="F295" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="G295" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="H295" s="22" t="s">
+        <v>514</v>
+      </c>
+      <c r="I295" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="J295" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="K295" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="L295" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="M295" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N295" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O295" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P295" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q295" s="22">
+        <v>1</v>
+      </c>
+      <c r="R295" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="296" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A296" s="26">
+        <v>2</v>
+      </c>
+      <c r="B296" s="26" t="s">
+        <v>500</v>
+      </c>
+      <c r="C296" s="26" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D296" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E296" s="26">
+        <v>1</v>
+      </c>
+      <c r="F296" s="27" t="s">
+        <v>525</v>
+      </c>
+      <c r="G296" s="26" t="s">
+        <v>526</v>
+      </c>
+      <c r="H296" s="26" t="s">
+        <v>527</v>
+      </c>
+      <c r="I296" s="26" t="s">
+        <v>528</v>
+      </c>
+      <c r="J296" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="K296" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="L296" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="M296" s="26" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N296" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O296" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P296" s="26" t="s">
+        <v>524</v>
+      </c>
+      <c r="Q296" s="26">
+        <v>1</v>
+      </c>
+      <c r="R296" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="297" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A297" s="32">
+        <v>2</v>
+      </c>
+      <c r="B297" s="32" t="s">
+        <v>500</v>
+      </c>
+      <c r="C297" s="32" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D297" s="32" t="s">
+        <v>539</v>
+      </c>
+      <c r="E297" s="32">
+        <v>1</v>
+      </c>
+      <c r="F297" s="33" t="s">
+        <v>540</v>
+      </c>
+      <c r="G297" s="32" t="s">
+        <v>541</v>
+      </c>
+      <c r="H297" s="32" t="s">
+        <v>542</v>
+      </c>
+      <c r="I297" s="32" t="s">
+        <v>543</v>
+      </c>
+      <c r="J297" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="K297" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="L297" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="M297" s="32" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N297" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O297" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P297" s="32" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q297" s="32">
+        <v>1</v>
+      </c>
+      <c r="R297" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="298" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A298" s="32">
+        <v>2</v>
+      </c>
+      <c r="B298" s="32" t="s">
+        <v>500</v>
+      </c>
+      <c r="C298" s="32" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D298" s="32" t="s">
+        <v>545</v>
+      </c>
+      <c r="E298" s="32">
+        <v>1</v>
+      </c>
+      <c r="F298" s="33" t="s">
+        <v>517</v>
+      </c>
+      <c r="G298" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="H298" s="32" t="s">
+        <v>518</v>
+      </c>
+      <c r="I298" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="J298" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="K298" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="L298" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="M298" s="32" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N298" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O298" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P298" s="32" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q298" s="32">
+        <v>1</v>
+      </c>
+      <c r="R298" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="299" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A299" s="26">
+        <v>1</v>
+      </c>
+      <c r="B299" s="26" t="s">
+        <v>500</v>
+      </c>
+      <c r="C299" s="26" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D299" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="E299" s="26">
+        <v>1</v>
+      </c>
+      <c r="F299" s="27" t="s">
+        <v>517</v>
+      </c>
+      <c r="G299" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H299" s="26" t="s">
+        <v>518</v>
+      </c>
+      <c r="I299" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="J299" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="K299" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="L299" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="M299" s="26" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N299" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O299" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P299" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q299" s="26">
+        <v>1</v>
+      </c>
+      <c r="R299" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="300" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A300" s="28">
+        <v>3</v>
+      </c>
+      <c r="B300" s="28" t="s">
+        <v>574</v>
+      </c>
+      <c r="C300" s="28" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D300" s="28" t="s">
+        <v>612</v>
+      </c>
+      <c r="E300" s="28">
+        <v>1</v>
+      </c>
+      <c r="F300" s="29" t="s">
+        <v>613</v>
+      </c>
+      <c r="G300" s="28" t="s">
+        <v>614</v>
+      </c>
+      <c r="H300" s="28" t="s">
+        <v>615</v>
+      </c>
+      <c r="I300" s="28" t="s">
+        <v>616</v>
+      </c>
+      <c r="J300" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="K300" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="L300" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="M300" s="28" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N300" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O300" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P300" s="28" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q300" s="28">
+        <v>1</v>
+      </c>
+      <c r="R300" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="301" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A301" s="22">
+        <v>3</v>
+      </c>
+      <c r="B301" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="C301" s="22" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D301" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="E301" s="22">
+        <v>1</v>
+      </c>
+      <c r="F301" s="23" t="s">
+        <v>619</v>
+      </c>
+      <c r="G301" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="H301" s="22" t="s">
+        <v>620</v>
+      </c>
+      <c r="I301" s="22" t="s">
+        <v>621</v>
+      </c>
+      <c r="J301" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="K301" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="L301" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="M301" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N301" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O301" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P301" s="22" t="s">
+        <v>617</v>
+      </c>
+      <c r="Q301" s="22">
+        <v>1</v>
+      </c>
+      <c r="R301" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="302" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A302" s="22">
+        <v>1</v>
+      </c>
+      <c r="B302" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="C302" s="22" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D302" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="E302" s="22">
+        <v>1</v>
+      </c>
+      <c r="F302" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="G302" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="H302" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="I302" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="J302" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K302" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L302" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="M302" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N302" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O302" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P302" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q302" s="22">
+        <v>1</v>
+      </c>
+      <c r="R302" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="303" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A303" s="28">
+        <v>1</v>
+      </c>
+      <c r="B303" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C303" s="28" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D303" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="E303" s="28">
+        <v>1</v>
+      </c>
+      <c r="F303" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="G303" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="H303" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="I303" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="J303" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K303" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L303" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="M303" s="28" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N303" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O303" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P303" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q303" s="28">
+        <v>1</v>
+      </c>
+      <c r="R303" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="304" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+      <c r="A304" s="30">
+        <v>1</v>
+      </c>
+      <c r="B304" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="C304" s="30" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D304" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="E304" s="30">
+        <v>1</v>
+      </c>
+      <c r="F304" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="G304" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="H304" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="I304" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="J304" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K304" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L304" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="M304" s="30" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N304" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O304" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="P304" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q304" s="30">
+        <v>1</v>
+      </c>
+      <c r="R304" s="30" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improve folder structure and updated schedules
</commit_message>
<xml_diff>
--- a/data/horarios/all.processed.xlsx
+++ b/data/horarios/all.processed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DACE1C-02E5-4A23-997A-C7DDAE763AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B332306-C860-43A6-B1DA-8800637CC451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3736" uniqueCount="1162">
   <si>
     <t>ciclo</t>
   </si>
@@ -3459,6 +3459,66 @@
   </si>
   <si>
     <t>C3S21111</t>
+  </si>
+  <si>
+    <t>C3P21321</t>
+  </si>
+  <si>
+    <t>C3P21322</t>
+  </si>
+  <si>
+    <t>C3P21323</t>
+  </si>
+  <si>
+    <t>C3P21324</t>
+  </si>
+  <si>
+    <t>C202A644</t>
+  </si>
+  <si>
+    <t>C202A643</t>
+  </si>
+  <si>
+    <t>C202A642</t>
+  </si>
+  <si>
+    <t>C202A641</t>
+  </si>
+  <si>
+    <t>C3P22334</t>
+  </si>
+  <si>
+    <t>C3P22313</t>
+  </si>
+  <si>
+    <t>C3P22312</t>
+  </si>
+  <si>
+    <t>C3P22311</t>
+  </si>
+  <si>
+    <t>C3P22333</t>
+  </si>
+  <si>
+    <t>C3P22332</t>
+  </si>
+  <si>
+    <t>C3P22331</t>
+  </si>
+  <si>
+    <t>C3P22324</t>
+  </si>
+  <si>
+    <t>C202B642</t>
+  </si>
+  <si>
+    <t>C3P21433</t>
+  </si>
+  <si>
+    <t>C3P21424</t>
+  </si>
+  <si>
+    <t>C3P21434</t>
   </si>
 </sst>
 </file>
@@ -3741,16 +3801,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R304" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="A1:R304" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}">
-    <filterColumn colId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R324" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="A1:R324" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}">
+    <filterColumn colId="1">
       <filters>
-        <filter val="FLORES"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="KONJA"/>
+        <filter val="MPAFC"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4055,10 +4110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R304"/>
+  <dimension ref="A1:R324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D305" sqref="D305"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E327" sqref="E327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5465,7 +5520,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -5976,106 +6031,106 @@
       <c r="R37" s="1"/>
     </row>
     <row r="38" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+      <c r="A38" s="3">
         <v>2</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="3">
         <v>2</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I38" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="K38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="L38" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="M38" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N38" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
+      <c r="M38" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
     </row>
     <row r="39" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+      <c r="A39" s="5">
         <v>4</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="E39" s="1">
-        <v>1</v>
-      </c>
-      <c r="F39" s="15" t="s">
+      <c r="E39" s="5">
+        <v>1</v>
+      </c>
+      <c r="F39" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I39" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="J39" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="K39" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="L39" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M39" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N39" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
+      <c r="M39" s="5" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
     </row>
     <row r="40" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
@@ -6180,55 +6235,55 @@
       <c r="R41" s="7"/>
     </row>
     <row r="42" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+      <c r="A42" s="6">
         <v>4</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E42" s="1">
-        <v>1</v>
-      </c>
-      <c r="F42" s="15" t="s">
+      <c r="E42" s="6">
+        <v>1</v>
+      </c>
+      <c r="F42" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I42" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J42" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="K42" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="L42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M42" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N42" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
+      <c r="M42" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
     </row>
     <row r="43" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
@@ -6435,55 +6490,55 @@
       <c r="R46" s="1"/>
     </row>
     <row r="47" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
+      <c r="A47" s="6">
         <v>2</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="6">
         <v>2</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="I47" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="J47" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="K47" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="L47" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M47" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N47" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
+      <c r="M47" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N47" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
     </row>
     <row r="48" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10">
@@ -6741,55 +6796,55 @@
       <c r="R52" s="1"/>
     </row>
     <row r="53" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
+      <c r="A53" s="5">
         <v>4</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="E53" s="1">
-        <v>1</v>
-      </c>
-      <c r="F53" s="15" t="s">
+      <c r="E53" s="5">
+        <v>1</v>
+      </c>
+      <c r="F53" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="G53" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="H53" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="I53" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="J53" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="K53" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L53" s="1" t="s">
+      <c r="L53" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M53" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N53" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
+      <c r="M53" s="5" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N53" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
     </row>
     <row r="54" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
@@ -6894,55 +6949,55 @@
       <c r="R55" s="1"/>
     </row>
     <row r="56" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
+      <c r="A56" s="12">
         <v>2</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="12">
         <v>2</v>
       </c>
-      <c r="F56" s="15" t="s">
+      <c r="F56" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="G56" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H56" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="I56" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="J56" s="1" t="s">
+      <c r="J56" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="K56" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L56" s="1" t="s">
+      <c r="L56" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="M56" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N56" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
+      <c r="M56" s="12" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N56" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O56" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
     </row>
     <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
@@ -6996,55 +7051,55 @@
       <c r="R57" s="1"/>
     </row>
     <row r="58" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
+      <c r="A58" s="4">
         <v>2</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="4">
         <v>2</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F58" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="G58" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="H58" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="I58" s="1" t="s">
+      <c r="I58" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="J58" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="K58" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="L58" s="1" t="s">
+      <c r="L58" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M58" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N58" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
+      <c r="M58" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N58" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
     </row>
     <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
@@ -10425,55 +10480,55 @@
       <c r="R124" s="1"/>
     </row>
     <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="1">
+      <c r="A125" s="3">
         <v>2</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D125" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E125" s="1">
-        <v>1</v>
-      </c>
-      <c r="F125" s="15" t="s">
+      <c r="E125" s="3">
+        <v>1</v>
+      </c>
+      <c r="F125" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="G125" s="1" t="s">
+      <c r="G125" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="H125" s="1" t="s">
+      <c r="H125" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="I125" s="1" t="s">
+      <c r="I125" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="J125" s="1" t="s">
+      <c r="J125" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="K125" s="1" t="s">
+      <c r="K125" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="L125" s="1" t="s">
+      <c r="L125" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="M125" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N125" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O125" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P125" s="1"/>
-      <c r="Q125" s="1"/>
-      <c r="R125" s="1"/>
+      <c r="M125" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N125" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O125" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P125" s="3"/>
+      <c r="Q125" s="3"/>
+      <c r="R125" s="3"/>
     </row>
     <row r="126" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
@@ -10731,50 +10786,50 @@
       <c r="R130" s="1"/>
     </row>
     <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="1">
+      <c r="A131" s="4">
         <v>3</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="D131" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E131" s="1">
-        <v>1</v>
-      </c>
-      <c r="F131" s="15" t="s">
+      <c r="E131" s="4">
+        <v>1</v>
+      </c>
+      <c r="F131" s="18" t="s">
         <v>607</v>
       </c>
-      <c r="G131" s="1" t="s">
+      <c r="G131" s="4" t="s">
         <v>608</v>
       </c>
-      <c r="H131" s="1" t="s">
+      <c r="H131" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="I131" s="1" t="s">
+      <c r="I131" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="J131" s="1" t="s">
+      <c r="J131" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="K131" s="1" t="s">
+      <c r="K131" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="L131" s="1" t="s">
+      <c r="L131" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="M131" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N131" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O131" s="1" t="s">
+      <c r="M131" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N131" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O131" s="4" t="s">
         <v>23</v>
       </c>
       <c r="P131" s="1"/>
@@ -10884,55 +10939,55 @@
       <c r="R133" s="4"/>
     </row>
     <row r="134" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="1">
+      <c r="A134" s="3">
         <v>3</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C134" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D134" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="E134" s="1">
-        <v>1</v>
-      </c>
-      <c r="F134" s="15" t="s">
+      <c r="E134" s="3">
+        <v>1</v>
+      </c>
+      <c r="F134" s="16" t="s">
         <v>624</v>
       </c>
-      <c r="G134" s="1" t="s">
+      <c r="G134" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="H134" s="1" t="s">
+      <c r="H134" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="I134" s="1" t="s">
+      <c r="I134" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="J134" s="1" t="s">
+      <c r="J134" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="K134" s="1" t="s">
+      <c r="K134" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="L134" s="1" t="s">
+      <c r="L134" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="M134" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N134" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O134" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P134" s="1"/>
-      <c r="Q134" s="1"/>
-      <c r="R134" s="1"/>
+      <c r="M134" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N134" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O134" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P134" s="3"/>
+      <c r="Q134" s="3"/>
+      <c r="R134" s="3"/>
     </row>
     <row r="135" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
@@ -11189,7 +11244,7 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>1</v>
       </c>
@@ -14420,7 +14475,7 @@
       <c r="Q202" s="1"/>
       <c r="R202" s="1"/>
     </row>
-    <row r="203" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>1</v>
       </c>
@@ -14471,7 +14526,7 @@
       <c r="Q203" s="1"/>
       <c r="R203" s="1"/>
     </row>
-    <row r="204" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>1</v>
       </c>
@@ -14522,7 +14577,7 @@
       <c r="Q204" s="1"/>
       <c r="R204" s="1"/>
     </row>
-    <row r="205" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>1</v>
       </c>
@@ -14573,7 +14628,7 @@
       <c r="Q205" s="1"/>
       <c r="R205" s="1"/>
     </row>
-    <row r="206" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>1</v>
       </c>
@@ -14624,7 +14679,7 @@
       <c r="Q206" s="1"/>
       <c r="R206" s="1"/>
     </row>
-    <row r="207" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>1</v>
       </c>
@@ -14675,7 +14730,7 @@
       <c r="Q207" s="1"/>
       <c r="R207" s="1"/>
     </row>
-    <row r="208" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>2</v>
       </c>
@@ -14726,7 +14781,7 @@
       <c r="Q208" s="1"/>
       <c r="R208" s="1"/>
     </row>
-    <row r="209" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>2</v>
       </c>
@@ -14777,7 +14832,7 @@
       <c r="Q209" s="1"/>
       <c r="R209" s="1"/>
     </row>
-    <row r="210" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>2</v>
       </c>
@@ -14828,7 +14883,7 @@
       <c r="Q210" s="1"/>
       <c r="R210" s="1"/>
     </row>
-    <row r="211" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>2</v>
       </c>
@@ -14879,7 +14934,7 @@
       <c r="Q211" s="1"/>
       <c r="R211" s="1"/>
     </row>
-    <row r="212" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>2</v>
       </c>
@@ -14930,7 +14985,7 @@
       <c r="Q212" s="1"/>
       <c r="R212" s="1"/>
     </row>
-    <row r="213" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>2</v>
       </c>
@@ -15753,106 +15808,106 @@
       <c r="R228" s="1"/>
     </row>
     <row r="229" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="1">
+      <c r="A229" s="4">
         <v>3</v>
       </c>
-      <c r="B229" s="1" t="s">
+      <c r="B229" s="4" t="s">
         <v>1006</v>
       </c>
-      <c r="C229" s="1" t="s">
+      <c r="C229" s="4" t="s">
         <v>1012</v>
       </c>
-      <c r="D229" s="1" t="s">
+      <c r="D229" s="4" t="s">
         <v>1013</v>
       </c>
-      <c r="E229" s="1">
-        <v>1</v>
-      </c>
-      <c r="F229" s="15" t="s">
+      <c r="E229" s="4">
+        <v>1</v>
+      </c>
+      <c r="F229" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="G229" s="1" t="s">
+      <c r="G229" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="H229" s="1" t="s">
+      <c r="H229" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="I229" s="1" t="s">
+      <c r="I229" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="J229" s="1" t="s">
+      <c r="J229" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K229" s="1" t="s">
+      <c r="K229" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L229" s="1" t="s">
+      <c r="L229" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M229" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N229" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O229" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P229" s="1"/>
-      <c r="Q229" s="1"/>
-      <c r="R229" s="1"/>
+      <c r="M229" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N229" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O229" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P229" s="4"/>
+      <c r="Q229" s="4"/>
+      <c r="R229" s="4"/>
     </row>
     <row r="230" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="1">
-        <v>1</v>
-      </c>
-      <c r="B230" s="1" t="s">
+      <c r="A230" s="3">
+        <v>1</v>
+      </c>
+      <c r="B230" s="3" t="s">
         <v>1006</v>
       </c>
-      <c r="C230" s="1" t="s">
+      <c r="C230" s="3" t="s">
         <v>1014</v>
       </c>
-      <c r="D230" s="1" t="s">
+      <c r="D230" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E230" s="1">
-        <v>1</v>
-      </c>
-      <c r="F230" s="15" t="s">
+      <c r="E230" s="3">
+        <v>1</v>
+      </c>
+      <c r="F230" s="16" t="s">
         <v>1015</v>
       </c>
-      <c r="G230" s="1" t="s">
+      <c r="G230" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="H230" s="1" t="s">
+      <c r="H230" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I230" s="1" t="s">
+      <c r="I230" s="3" t="s">
         <v>1017</v>
       </c>
-      <c r="J230" s="1" t="s">
+      <c r="J230" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K230" s="1" t="s">
+      <c r="K230" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L230" s="1" t="s">
+      <c r="L230" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M230" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N230" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O230" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P230" s="1"/>
-      <c r="Q230" s="1"/>
-      <c r="R230" s="1"/>
+      <c r="M230" s="3" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N230" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O230" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P230" s="3"/>
+      <c r="Q230" s="3"/>
+      <c r="R230" s="3"/>
     </row>
     <row r="231" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
@@ -16008,55 +16063,55 @@
       <c r="R233" s="1"/>
     </row>
     <row r="234" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="1">
-        <v>1</v>
-      </c>
-      <c r="B234" s="1" t="s">
+      <c r="A234" s="4">
+        <v>1</v>
+      </c>
+      <c r="B234" s="4" t="s">
         <v>1006</v>
       </c>
-      <c r="C234" s="1" t="s">
+      <c r="C234" s="4" t="s">
         <v>1032</v>
       </c>
-      <c r="D234" s="1" t="s">
+      <c r="D234" s="4" t="s">
         <v>1033</v>
       </c>
-      <c r="E234" s="1">
-        <v>1</v>
-      </c>
-      <c r="F234" s="15" t="s">
+      <c r="E234" s="4">
+        <v>1</v>
+      </c>
+      <c r="F234" s="18" t="s">
         <v>475</v>
       </c>
-      <c r="G234" s="1" t="s">
+      <c r="G234" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="H234" s="1" t="s">
+      <c r="H234" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="I234" s="1" t="s">
+      <c r="I234" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="J234" s="1" t="s">
+      <c r="J234" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K234" s="1" t="s">
+      <c r="K234" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L234" s="1" t="s">
+      <c r="L234" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M234" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N234" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O234" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P234" s="1"/>
-      <c r="Q234" s="1"/>
-      <c r="R234" s="1"/>
+      <c r="M234" s="4" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N234" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O234" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P234" s="4"/>
+      <c r="Q234" s="4"/>
+      <c r="R234" s="4"/>
     </row>
     <row r="235" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
@@ -16263,157 +16318,157 @@
       <c r="R238" s="1"/>
     </row>
     <row r="239" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="1">
+      <c r="A239" s="6">
         <v>3</v>
       </c>
-      <c r="B239" s="1" t="s">
+      <c r="B239" s="6" t="s">
         <v>1006</v>
       </c>
-      <c r="C239" s="1" t="s">
+      <c r="C239" s="6" t="s">
         <v>1050</v>
       </c>
-      <c r="D239" s="1" t="s">
+      <c r="D239" s="6" t="s">
         <v>1051</v>
       </c>
-      <c r="E239" s="1">
-        <v>1</v>
-      </c>
-      <c r="F239" s="15" t="s">
+      <c r="E239" s="6">
+        <v>1</v>
+      </c>
+      <c r="F239" s="13" t="s">
         <v>1052</v>
       </c>
-      <c r="G239" s="1" t="s">
+      <c r="G239" s="6" t="s">
         <v>1053</v>
       </c>
-      <c r="H239" s="1" t="s">
+      <c r="H239" s="6" t="s">
         <v>1054</v>
       </c>
-      <c r="I239" s="1" t="s">
+      <c r="I239" s="6" t="s">
         <v>1055</v>
       </c>
-      <c r="J239" s="1" t="s">
+      <c r="J239" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K239" s="1" t="s">
+      <c r="K239" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L239" s="1" t="s">
+      <c r="L239" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M239" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N239" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O239" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P239" s="1"/>
-      <c r="Q239" s="1"/>
-      <c r="R239" s="1"/>
+      <c r="M239" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N239" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O239" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P239" s="6"/>
+      <c r="Q239" s="6"/>
+      <c r="R239" s="6"/>
     </row>
     <row r="240" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="1">
-        <v>1</v>
-      </c>
-      <c r="B240" s="1" t="s">
+      <c r="A240" s="5">
+        <v>1</v>
+      </c>
+      <c r="B240" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="C240" s="1" t="s">
+      <c r="C240" s="5" t="s">
         <v>1056</v>
       </c>
-      <c r="D240" s="1" t="s">
+      <c r="D240" s="5" t="s">
         <v>1057</v>
       </c>
-      <c r="E240" s="1">
-        <v>1</v>
-      </c>
-      <c r="F240" s="15" t="s">
+      <c r="E240" s="5">
+        <v>1</v>
+      </c>
+      <c r="F240" s="19" t="s">
         <v>1058</v>
       </c>
-      <c r="G240" s="1" t="s">
+      <c r="G240" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="H240" s="1" t="s">
+      <c r="H240" s="5" t="s">
         <v>1059</v>
       </c>
-      <c r="I240" s="1" t="s">
+      <c r="I240" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="J240" s="1" t="s">
+      <c r="J240" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K240" s="1" t="s">
+      <c r="K240" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="L240" s="1" t="s">
+      <c r="L240" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M240" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N240" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O240" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P240" s="1"/>
-      <c r="Q240" s="1"/>
-      <c r="R240" s="1"/>
+      <c r="M240" s="5" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N240" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O240" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P240" s="5"/>
+      <c r="Q240" s="5"/>
+      <c r="R240" s="5"/>
     </row>
     <row r="241" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="1">
+      <c r="A241" s="10">
         <v>2</v>
       </c>
-      <c r="B241" s="1" t="s">
+      <c r="B241" s="10" t="s">
         <v>1006</v>
       </c>
-      <c r="C241" s="1" t="s">
+      <c r="C241" s="10" t="s">
         <v>1061</v>
       </c>
-      <c r="D241" s="1" t="s">
+      <c r="D241" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E241" s="1">
-        <v>1</v>
-      </c>
-      <c r="F241" s="15" t="s">
+      <c r="E241" s="10">
+        <v>1</v>
+      </c>
+      <c r="F241" s="20" t="s">
         <v>1062</v>
       </c>
-      <c r="G241" s="1" t="s">
+      <c r="G241" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="H241" s="1" t="s">
+      <c r="H241" s="10" t="s">
         <v>1063</v>
       </c>
-      <c r="I241" s="1" t="s">
+      <c r="I241" s="10" t="s">
         <v>1064</v>
       </c>
-      <c r="J241" s="1" t="s">
+      <c r="J241" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K241" s="1" t="s">
+      <c r="K241" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="L241" s="1" t="s">
+      <c r="L241" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M241" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N241" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O241" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P241" s="1"/>
-      <c r="Q241" s="1"/>
-      <c r="R241" s="1"/>
+      <c r="M241" s="10" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N241" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O241" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P241" s="10"/>
+      <c r="Q241" s="10"/>
+      <c r="R241" s="10"/>
     </row>
     <row r="242" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
@@ -16467,55 +16522,55 @@
       <c r="R242" s="1"/>
     </row>
     <row r="243" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A243" s="1">
+      <c r="A243" s="10">
         <v>3</v>
       </c>
-      <c r="B243" s="1" t="s">
+      <c r="B243" s="10" t="s">
         <v>1006</v>
       </c>
-      <c r="C243" s="1" t="s">
+      <c r="C243" s="10" t="s">
         <v>1069</v>
       </c>
-      <c r="D243" s="1" t="s">
+      <c r="D243" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E243" s="1">
-        <v>1</v>
-      </c>
-      <c r="F243" s="15" t="s">
+      <c r="E243" s="10">
+        <v>1</v>
+      </c>
+      <c r="F243" s="20" t="s">
         <v>1070</v>
       </c>
-      <c r="G243" s="1" t="s">
+      <c r="G243" s="10" t="s">
         <v>1071</v>
       </c>
-      <c r="H243" s="1" t="s">
+      <c r="H243" s="10" t="s">
         <v>1072</v>
       </c>
-      <c r="I243" s="1" t="s">
+      <c r="I243" s="10" t="s">
         <v>1073</v>
       </c>
-      <c r="J243" s="1" t="s">
+      <c r="J243" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K243" s="1" t="s">
+      <c r="K243" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="L243" s="1" t="s">
+      <c r="L243" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M243" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N243" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O243" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P243" s="1"/>
-      <c r="Q243" s="1"/>
-      <c r="R243" s="1"/>
+      <c r="M243" s="10" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N243" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O243" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P243" s="10"/>
+      <c r="Q243" s="10"/>
+      <c r="R243" s="10"/>
     </row>
     <row r="244" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
@@ -16569,55 +16624,55 @@
       <c r="R244" s="1"/>
     </row>
     <row r="245" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A245" s="1">
+      <c r="A245" s="10">
         <v>4</v>
       </c>
-      <c r="B245" s="1" t="s">
+      <c r="B245" s="10" t="s">
         <v>1006</v>
       </c>
-      <c r="C245" s="1" t="s">
+      <c r="C245" s="10" t="s">
         <v>1078</v>
       </c>
-      <c r="D245" s="1" t="s">
+      <c r="D245" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="E245" s="1">
-        <v>1</v>
-      </c>
-      <c r="F245" s="15" t="s">
+      <c r="E245" s="10">
+        <v>1</v>
+      </c>
+      <c r="F245" s="20" t="s">
         <v>1079</v>
       </c>
-      <c r="G245" s="1" t="s">
+      <c r="G245" s="10" t="s">
         <v>1080</v>
       </c>
-      <c r="H245" s="1" t="s">
+      <c r="H245" s="10" t="s">
         <v>1081</v>
       </c>
-      <c r="I245" s="1" t="s">
+      <c r="I245" s="10" t="s">
         <v>1082</v>
       </c>
-      <c r="J245" s="1" t="s">
+      <c r="J245" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K245" s="1" t="s">
+      <c r="K245" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="L245" s="1" t="s">
+      <c r="L245" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M245" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N245" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O245" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P245" s="1"/>
-      <c r="Q245" s="1"/>
-      <c r="R245" s="1"/>
+      <c r="M245" s="10" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N245" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O245" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P245" s="10"/>
+      <c r="Q245" s="10"/>
+      <c r="R245" s="10"/>
     </row>
     <row r="246" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
@@ -16671,55 +16726,55 @@
       <c r="R246" s="1"/>
     </row>
     <row r="247" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A247" s="1">
+      <c r="A247" s="6">
         <v>3</v>
       </c>
-      <c r="B247" s="1" t="s">
+      <c r="B247" s="6" t="s">
         <v>1006</v>
       </c>
-      <c r="C247" s="1" t="s">
+      <c r="C247" s="6" t="s">
         <v>1087</v>
       </c>
-      <c r="D247" s="1" t="s">
+      <c r="D247" s="6" t="s">
         <v>1088</v>
       </c>
-      <c r="E247" s="1">
-        <v>1</v>
-      </c>
-      <c r="F247" s="15" t="s">
+      <c r="E247" s="6">
+        <v>1</v>
+      </c>
+      <c r="F247" s="13" t="s">
         <v>494</v>
       </c>
-      <c r="G247" s="1" t="s">
+      <c r="G247" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="H247" s="1" t="s">
+      <c r="H247" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="I247" s="1" t="s">
+      <c r="I247" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="J247" s="1" t="s">
+      <c r="J247" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K247" s="1" t="s">
+      <c r="K247" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L247" s="1" t="s">
+      <c r="L247" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M247" s="1" t="b">
-        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
-        <v>0</v>
-      </c>
-      <c r="N247" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="O247" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P247" s="1"/>
-      <c r="Q247" s="1"/>
-      <c r="R247" s="1"/>
+      <c r="M247" s="6" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N247" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O247" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P247" s="6"/>
+      <c r="Q247" s="6"/>
+      <c r="R247" s="6"/>
     </row>
     <row r="248" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="5">
@@ -18032,7 +18087,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="271" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A271" s="5">
         <v>1</v>
       </c>
@@ -18089,7 +18144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="272" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A272" s="5">
         <v>1</v>
       </c>
@@ -18146,7 +18201,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="273" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>1</v>
       </c>
@@ -19967,6 +20022,1146 @@
         <v>1</v>
       </c>
       <c r="R304" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="305" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A305" s="24">
+        <v>2</v>
+      </c>
+      <c r="B305" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="C305" s="24" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D305" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="E305" s="24">
+        <v>2</v>
+      </c>
+      <c r="F305" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="G305" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="H305" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="I305" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="J305" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K305" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="L305" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="M305" s="24" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N305" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O305" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P305" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q305" s="24">
+        <v>2</v>
+      </c>
+      <c r="R305" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="306" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A306" s="26">
+        <v>2</v>
+      </c>
+      <c r="B306" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C306" s="26" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D306" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="E306" s="26">
+        <v>2</v>
+      </c>
+      <c r="F306" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="G306" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="H306" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="I306" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="J306" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K306" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L306" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M306" s="26" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N306" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O306" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P306" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q306" s="26">
+        <v>2</v>
+      </c>
+      <c r="R306" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="307" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A307" s="30">
+        <v>2</v>
+      </c>
+      <c r="B307" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="C307" s="30" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D307" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="E307" s="30">
+        <v>2</v>
+      </c>
+      <c r="F307" s="31" t="s">
+        <v>283</v>
+      </c>
+      <c r="G307" s="30" t="s">
+        <v>284</v>
+      </c>
+      <c r="H307" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="I307" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="J307" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="K307" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="L307" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="M307" s="30" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N307" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O307" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="P307" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q307" s="30">
+        <v>2</v>
+      </c>
+      <c r="R307" s="30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="308" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A308" s="22">
+        <v>2</v>
+      </c>
+      <c r="B308" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="C308" s="22" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D308" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E308" s="22">
+        <v>2</v>
+      </c>
+      <c r="F308" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="G308" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="H308" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="I308" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="J308" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K308" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="L308" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M308" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N308" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O308" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P308" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q308" s="22">
+        <v>2</v>
+      </c>
+      <c r="R308" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="309" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A309" s="32">
+        <v>4</v>
+      </c>
+      <c r="B309" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C309" s="32" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D309" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="E309" s="32">
+        <v>1</v>
+      </c>
+      <c r="F309" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="G309" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="H309" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="I309" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="J309" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K309" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L309" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="M309" s="32" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N309" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O309" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P309" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q309" s="32">
+        <v>1</v>
+      </c>
+      <c r="R309" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="310" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A310" s="22">
+        <v>4</v>
+      </c>
+      <c r="B310" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="C310" s="22" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D310" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="E310" s="22">
+        <v>1</v>
+      </c>
+      <c r="F310" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="G310" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H310" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I310" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="J310" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K310" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="L310" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M310" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N310" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O310" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P310" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q310" s="22">
+        <v>1</v>
+      </c>
+      <c r="R310" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="311" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A311" s="32">
+        <v>4</v>
+      </c>
+      <c r="B311" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C311" s="32" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D311" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="E311" s="32">
+        <v>1</v>
+      </c>
+      <c r="F311" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="G311" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="H311" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="I311" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="J311" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K311" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L311" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="M311" s="32" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N311" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O311" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P311" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q311" s="32">
+        <v>1</v>
+      </c>
+      <c r="R311" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="312" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A312" s="26">
+        <v>4</v>
+      </c>
+      <c r="B312" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C312" s="26" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D312" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="E312" s="26">
+        <v>1</v>
+      </c>
+      <c r="F312" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="G312" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="H312" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I312" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="J312" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K312" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L312" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M312" s="26" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N312" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O312" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P312" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q312" s="26">
+        <v>1</v>
+      </c>
+      <c r="R312" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="313" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A313" s="28">
+        <v>3</v>
+      </c>
+      <c r="B313" s="28" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C313" s="28" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D313" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E313" s="28">
+        <v>1</v>
+      </c>
+      <c r="F313" s="29" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G313" s="28" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H313" s="28" t="s">
+        <v>1072</v>
+      </c>
+      <c r="I313" s="28" t="s">
+        <v>1073</v>
+      </c>
+      <c r="J313" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K313" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="L313" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="M313" s="28" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N313" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O313" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P313" s="28" t="s">
+        <v>1069</v>
+      </c>
+      <c r="Q313" s="28">
+        <v>1</v>
+      </c>
+      <c r="R313" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="314" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A314" s="32">
+        <v>1</v>
+      </c>
+      <c r="B314" s="32" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C314" s="32" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D314" s="32" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E314" s="32">
+        <v>1</v>
+      </c>
+      <c r="F314" s="33" t="s">
+        <v>1058</v>
+      </c>
+      <c r="G314" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="H314" s="32" t="s">
+        <v>1059</v>
+      </c>
+      <c r="I314" s="32" t="s">
+        <v>1060</v>
+      </c>
+      <c r="J314" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K314" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="L314" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="M314" s="32" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N314" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O314" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P314" s="32" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Q314" s="32">
+        <v>1</v>
+      </c>
+      <c r="R314" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="315" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A315" s="22">
+        <v>1</v>
+      </c>
+      <c r="B315" s="22" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C315" s="22" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D315" s="22" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E315" s="22">
+        <v>1</v>
+      </c>
+      <c r="F315" s="23" t="s">
+        <v>475</v>
+      </c>
+      <c r="G315" s="22" t="s">
+        <v>476</v>
+      </c>
+      <c r="H315" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="I315" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="J315" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K315" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L315" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="M315" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N315" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O315" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P315" s="22" t="s">
+        <v>1032</v>
+      </c>
+      <c r="Q315" s="22">
+        <v>1</v>
+      </c>
+      <c r="R315" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="316" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A316" s="24">
+        <v>1</v>
+      </c>
+      <c r="B316" s="24" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C316" s="24" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D316" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E316" s="24">
+        <v>1</v>
+      </c>
+      <c r="F316" s="25" t="s">
+        <v>1015</v>
+      </c>
+      <c r="G316" s="24" t="s">
+        <v>1016</v>
+      </c>
+      <c r="H316" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I316" s="24" t="s">
+        <v>1017</v>
+      </c>
+      <c r="J316" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K316" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L316" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M316" s="24" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N316" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O316" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P316" s="24" t="s">
+        <v>1014</v>
+      </c>
+      <c r="Q316" s="24">
+        <v>1</v>
+      </c>
+      <c r="R316" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="317" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A317" s="26">
+        <v>3</v>
+      </c>
+      <c r="B317" s="26" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C317" s="26" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D317" s="26" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E317" s="26">
+        <v>1</v>
+      </c>
+      <c r="F317" s="27" t="s">
+        <v>1052</v>
+      </c>
+      <c r="G317" s="26" t="s">
+        <v>1053</v>
+      </c>
+      <c r="H317" s="26" t="s">
+        <v>1054</v>
+      </c>
+      <c r="I317" s="26" t="s">
+        <v>1055</v>
+      </c>
+      <c r="J317" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K317" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L317" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M317" s="26" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N317" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O317" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P317" s="26" t="s">
+        <v>1050</v>
+      </c>
+      <c r="Q317" s="26">
+        <v>1</v>
+      </c>
+      <c r="R317" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="318" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A318" s="22">
+        <v>3</v>
+      </c>
+      <c r="B318" s="22" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C318" s="22" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D318" s="22" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E318" s="22">
+        <v>1</v>
+      </c>
+      <c r="F318" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="G318" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="H318" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="I318" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="J318" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K318" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="L318" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="M318" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N318" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O318" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P318" s="22" t="s">
+        <v>1012</v>
+      </c>
+      <c r="Q318" s="22">
+        <v>1</v>
+      </c>
+      <c r="R318" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="319" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A319" s="26">
+        <v>3</v>
+      </c>
+      <c r="B319" s="26" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C319" s="26" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D319" s="26" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E319" s="26">
+        <v>1</v>
+      </c>
+      <c r="F319" s="27" t="s">
+        <v>494</v>
+      </c>
+      <c r="G319" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="H319" s="26" t="s">
+        <v>496</v>
+      </c>
+      <c r="I319" s="26" t="s">
+        <v>497</v>
+      </c>
+      <c r="J319" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K319" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L319" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M319" s="26" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N319" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O319" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P319" s="26" t="s">
+        <v>1087</v>
+      </c>
+      <c r="Q319" s="26">
+        <v>1</v>
+      </c>
+      <c r="R319" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="320" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A320" s="28">
+        <v>2</v>
+      </c>
+      <c r="B320" s="28" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C320" s="28" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D320" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E320" s="28">
+        <v>1</v>
+      </c>
+      <c r="F320" s="29" t="s">
+        <v>1062</v>
+      </c>
+      <c r="G320" s="28" t="s">
+        <v>801</v>
+      </c>
+      <c r="H320" s="28" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I320" s="28" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J320" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K320" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="L320" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="M320" s="28" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N320" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O320" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P320" s="28" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Q320" s="28">
+        <v>1</v>
+      </c>
+      <c r="R320" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="321" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A321" s="28">
+        <v>4</v>
+      </c>
+      <c r="B321" s="28" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C321" s="28" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D321" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E321" s="28">
+        <v>1</v>
+      </c>
+      <c r="F321" s="29" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G321" s="28" t="s">
+        <v>1080</v>
+      </c>
+      <c r="H321" s="28" t="s">
+        <v>1081</v>
+      </c>
+      <c r="I321" s="28" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J321" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K321" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="L321" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="M321" s="28" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N321" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O321" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P321" s="28" t="s">
+        <v>1078</v>
+      </c>
+      <c r="Q321" s="28">
+        <v>1</v>
+      </c>
+      <c r="R321" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="322" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A322" s="24">
+        <v>3</v>
+      </c>
+      <c r="B322" s="24" t="s">
+        <v>574</v>
+      </c>
+      <c r="C322" s="24" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D322" s="24" t="s">
+        <v>623</v>
+      </c>
+      <c r="E322" s="24">
+        <v>1</v>
+      </c>
+      <c r="F322" s="25" t="s">
+        <v>624</v>
+      </c>
+      <c r="G322" s="24" t="s">
+        <v>625</v>
+      </c>
+      <c r="H322" s="24" t="s">
+        <v>626</v>
+      </c>
+      <c r="I322" s="24" t="s">
+        <v>627</v>
+      </c>
+      <c r="J322" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="K322" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="L322" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="M322" s="24" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N322" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="O322" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P322" s="24" t="s">
+        <v>622</v>
+      </c>
+      <c r="Q322" s="24">
+        <v>1</v>
+      </c>
+      <c r="R322" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="323" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A323" s="24">
+        <v>2</v>
+      </c>
+      <c r="B323" s="24" t="s">
+        <v>574</v>
+      </c>
+      <c r="C323" s="24" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D323" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E323" s="24">
+        <v>1</v>
+      </c>
+      <c r="F323" s="25" t="s">
+        <v>585</v>
+      </c>
+      <c r="G323" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="H323" s="24" t="s">
+        <v>586</v>
+      </c>
+      <c r="I323" s="24" t="s">
+        <v>587</v>
+      </c>
+      <c r="J323" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="K323" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="L323" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="M323" s="24" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N323" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="O323" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P323" s="24" t="s">
+        <v>584</v>
+      </c>
+      <c r="Q323" s="24">
+        <v>1</v>
+      </c>
+      <c r="R323" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="324" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A324" s="22">
+        <v>3</v>
+      </c>
+      <c r="B324" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="C324" s="22" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D324" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E324" s="22">
+        <v>1</v>
+      </c>
+      <c r="F324" s="23" t="s">
+        <v>607</v>
+      </c>
+      <c r="G324" s="22" t="s">
+        <v>608</v>
+      </c>
+      <c r="H324" s="22" t="s">
+        <v>609</v>
+      </c>
+      <c r="I324" s="22" t="s">
+        <v>610</v>
+      </c>
+      <c r="J324" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="K324" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="L324" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="M324" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>1</v>
+      </c>
+      <c r="N324" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O324" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P324" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="Q324" s="22">
+        <v>1</v>
+      </c>
+      <c r="R324" s="22" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated data and improve folder structure
</commit_message>
<xml_diff>
--- a/data/horarios/all.processed.xlsx
+++ b/data/horarios/all.processed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B332306-C860-43A6-B1DA-8800637CC451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC656C3-E4A2-469C-96DC-FF7245E74642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3736" uniqueCount="1162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3769" uniqueCount="1174">
   <si>
     <t>ciclo</t>
   </si>
@@ -3519,6 +3519,42 @@
   </si>
   <si>
     <t>C3P21434</t>
+  </si>
+  <si>
+    <t>C2S20324</t>
+  </si>
+  <si>
+    <t>SEMINARIO DE HERRAMIENTAS DE INVESTIGACION</t>
+  </si>
+  <si>
+    <t>MERR910518NZ3</t>
+  </si>
+  <si>
+    <t>Mendoza</t>
+  </si>
+  <si>
+    <t>Rivera</t>
+  </si>
+  <si>
+    <t>Ricardo Jacob</t>
+  </si>
+  <si>
+    <t>C3S21411</t>
+  </si>
+  <si>
+    <t>CONTABILIDAD GERENCIAL Y DE GESTION</t>
+  </si>
+  <si>
+    <t>C3S20811</t>
+  </si>
+  <si>
+    <t>10147714</t>
+  </si>
+  <si>
+    <t>NAVARRO</t>
+  </si>
+  <si>
+    <t>BALDEON DE COTRINA</t>
   </si>
 </sst>
 </file>
@@ -3801,14 +3837,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R324" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="A1:R324" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="MPAFC"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}" name="Table1" displayName="Table1" ref="A1:R327" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="A1:R327" xr:uid="{AD5A41C9-0974-4406-8AD1-3051A248D85D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A144:R214">
     <sortCondition ref="C1:C274"/>
   </sortState>
@@ -4110,10 +4140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R324"/>
+  <dimension ref="A1:R327"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E327" sqref="E327"/>
+    <sheetView tabSelected="1" topLeftCell="A311" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A325" sqref="A325:A327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4194,7 +4224,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -4245,7 +4275,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>4</v>
       </c>
@@ -4296,7 +4326,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4347,7 +4377,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4398,7 +4428,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -4449,7 +4479,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -4500,7 +4530,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -4551,7 +4581,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -4602,7 +4632,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -4653,7 +4683,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -4704,7 +4734,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -4755,7 +4785,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -4806,7 +4836,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -4857,7 +4887,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -4908,7 +4938,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -4959,7 +4989,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>3</v>
       </c>
@@ -5010,7 +5040,7 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
     </row>
-    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>4</v>
       </c>
@@ -5061,7 +5091,7 @@
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
     </row>
-    <row r="19" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -5112,7 +5142,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -5163,7 +5193,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>3</v>
       </c>
@@ -5214,7 +5244,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -5265,7 +5295,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -5316,7 +5346,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -5367,7 +5397,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -5418,7 +5448,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -5469,7 +5499,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -5520,7 +5550,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -5571,7 +5601,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>3</v>
       </c>
@@ -5622,7 +5652,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -5673,7 +5703,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -5724,7 +5754,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>4</v>
       </c>
@@ -5775,7 +5805,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2</v>
       </c>
@@ -5826,7 +5856,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>4</v>
       </c>
@@ -5877,7 +5907,7 @@
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
     </row>
-    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>3</v>
       </c>
@@ -5928,7 +5958,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -5979,7 +6009,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2</v>
       </c>
@@ -6030,7 +6060,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>2</v>
       </c>
@@ -6081,7 +6111,7 @@
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
     </row>
-    <row r="39" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>4</v>
       </c>
@@ -6132,7 +6162,7 @@
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
     </row>
-    <row r="40" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>3</v>
       </c>
@@ -6183,7 +6213,7 @@
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
     </row>
-    <row r="41" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>3</v>
       </c>
@@ -6234,7 +6264,7 @@
       <c r="Q41" s="7"/>
       <c r="R41" s="7"/>
     </row>
-    <row r="42" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>4</v>
       </c>
@@ -6285,7 +6315,7 @@
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
     </row>
-    <row r="43" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>1</v>
       </c>
@@ -6336,7 +6366,7 @@
       <c r="Q43" s="12"/>
       <c r="R43" s="12"/>
     </row>
-    <row r="44" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>3</v>
       </c>
@@ -6387,7 +6417,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>3</v>
       </c>
@@ -6438,7 +6468,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2</v>
       </c>
@@ -6489,7 +6519,7 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>2</v>
       </c>
@@ -6540,7 +6570,7 @@
       <c r="Q47" s="6"/>
       <c r="R47" s="6"/>
     </row>
-    <row r="48" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A48" s="10">
         <v>1</v>
       </c>
@@ -6591,7 +6621,7 @@
       <c r="Q48" s="10"/>
       <c r="R48" s="10"/>
     </row>
-    <row r="49" spans="1:18" ht="66" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -6642,7 +6672,7 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
     </row>
-    <row r="50" spans="1:18" ht="66" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>3</v>
       </c>
@@ -6693,7 +6723,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>1</v>
       </c>
@@ -6744,7 +6774,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
     </row>
-    <row r="52" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>1</v>
       </c>
@@ -6795,7 +6825,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>4</v>
       </c>
@@ -6846,7 +6876,7 @@
       <c r="Q53" s="5"/>
       <c r="R53" s="5"/>
     </row>
-    <row r="54" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>1</v>
       </c>
@@ -6897,7 +6927,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2</v>
       </c>
@@ -6948,7 +6978,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A56" s="12">
         <v>2</v>
       </c>
@@ -6999,7 +7029,7 @@
       <c r="Q56" s="12"/>
       <c r="R56" s="12"/>
     </row>
-    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2</v>
       </c>
@@ -7050,7 +7080,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
     </row>
-    <row r="58" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>2</v>
       </c>
@@ -7101,7 +7131,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>3</v>
       </c>
@@ -7152,7 +7182,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>3</v>
       </c>
@@ -7203,7 +7233,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>3</v>
       </c>
@@ -7254,7 +7284,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>4</v>
       </c>
@@ -7305,7 +7335,7 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
     </row>
-    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>4</v>
       </c>
@@ -7362,7 +7392,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>1</v>
       </c>
@@ -7413,7 +7443,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>1</v>
       </c>
@@ -7464,7 +7494,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="12">
         <v>1</v>
       </c>
@@ -7515,7 +7545,7 @@
       <c r="Q66" s="12"/>
       <c r="R66" s="12"/>
     </row>
-    <row r="67" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>1</v>
       </c>
@@ -7566,7 +7596,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>1</v>
       </c>
@@ -7617,7 +7647,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>1</v>
       </c>
@@ -7668,7 +7698,7 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2</v>
       </c>
@@ -7719,7 +7749,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2</v>
       </c>
@@ -7770,7 +7800,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2</v>
       </c>
@@ -7821,7 +7851,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2</v>
       </c>
@@ -7872,7 +7902,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>3</v>
       </c>
@@ -7923,7 +7953,7 @@
       <c r="Q74" s="6"/>
       <c r="R74" s="6"/>
     </row>
-    <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>3</v>
       </c>
@@ -7974,7 +8004,7 @@
       <c r="Q75" s="5"/>
       <c r="R75" s="5"/>
     </row>
-    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>3</v>
       </c>
@@ -8025,7 +8055,7 @@
       <c r="Q76" s="3"/>
       <c r="R76" s="3"/>
     </row>
-    <row r="77" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>3</v>
       </c>
@@ -8076,7 +8106,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A78" s="10">
         <v>3</v>
       </c>
@@ -8127,7 +8157,7 @@
       <c r="Q78" s="10"/>
       <c r="R78" s="10"/>
     </row>
-    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>4</v>
       </c>
@@ -8178,7 +8208,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>4</v>
       </c>
@@ -8229,7 +8259,7 @@
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
     </row>
-    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>4</v>
       </c>
@@ -8280,7 +8310,7 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <v>4</v>
       </c>
@@ -8331,7 +8361,7 @@
       <c r="Q82" s="6"/>
       <c r="R82" s="6"/>
     </row>
-    <row r="83" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>1</v>
       </c>
@@ -8382,7 +8412,7 @@
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>1</v>
       </c>
@@ -8433,7 +8463,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>1</v>
       </c>
@@ -8484,7 +8514,7 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>1</v>
       </c>
@@ -8535,7 +8565,7 @@
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
     </row>
-    <row r="87" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>1</v>
       </c>
@@ -8586,7 +8616,7 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>2</v>
       </c>
@@ -8637,7 +8667,7 @@
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
     </row>
-    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>2</v>
       </c>
@@ -8688,7 +8718,7 @@
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>2</v>
       </c>
@@ -8739,7 +8769,7 @@
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>3</v>
       </c>
@@ -8790,7 +8820,7 @@
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>3</v>
       </c>
@@ -8841,7 +8871,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>3</v>
       </c>
@@ -8892,7 +8922,7 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>3</v>
       </c>
@@ -8943,7 +8973,7 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>3</v>
       </c>
@@ -8994,7 +9024,7 @@
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>3</v>
       </c>
@@ -9045,7 +9075,7 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
     </row>
-    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>4</v>
       </c>
@@ -9096,7 +9126,7 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>4</v>
       </c>
@@ -9147,7 +9177,7 @@
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>4</v>
       </c>
@@ -9198,7 +9228,7 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>4</v>
       </c>
@@ -9249,7 +9279,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>4</v>
       </c>
@@ -9300,7 +9330,7 @@
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
     </row>
-    <row r="102" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>1</v>
       </c>
@@ -9351,7 +9381,7 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
     </row>
-    <row r="103" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>1</v>
       </c>
@@ -9402,7 +9432,7 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>1</v>
       </c>
@@ -9453,7 +9483,7 @@
       <c r="Q104" s="4"/>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105" s="6">
         <v>1</v>
       </c>
@@ -9504,7 +9534,7 @@
       <c r="Q105" s="6"/>
       <c r="R105" s="6"/>
     </row>
-    <row r="106" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>1</v>
       </c>
@@ -9555,7 +9585,7 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="6">
         <v>2</v>
       </c>
@@ -9606,7 +9636,7 @@
       <c r="Q107" s="6"/>
       <c r="R107" s="6"/>
     </row>
-    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>2</v>
       </c>
@@ -9657,7 +9687,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>2</v>
       </c>
@@ -9708,7 +9738,7 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>2</v>
       </c>
@@ -9759,7 +9789,7 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A111" s="5">
         <v>2</v>
       </c>
@@ -9810,7 +9840,7 @@
       <c r="Q111" s="5"/>
       <c r="R111" s="5"/>
     </row>
-    <row r="112" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A112" s="5">
         <v>2</v>
       </c>
@@ -9861,7 +9891,7 @@
       <c r="Q112" s="5"/>
       <c r="R112" s="5"/>
     </row>
-    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="12">
         <v>3</v>
       </c>
@@ -9912,7 +9942,7 @@
       <c r="Q113" s="12"/>
       <c r="R113" s="12"/>
     </row>
-    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="12">
         <v>3</v>
       </c>
@@ -9963,7 +9993,7 @@
       <c r="Q114" s="12"/>
       <c r="R114" s="12"/>
     </row>
-    <row r="115" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A115" s="5">
         <v>3</v>
       </c>
@@ -10014,7 +10044,7 @@
       <c r="Q115" s="5"/>
       <c r="R115" s="5"/>
     </row>
-    <row r="116" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A116" s="6">
         <v>3</v>
       </c>
@@ -10065,7 +10095,7 @@
       <c r="Q116" s="6"/>
       <c r="R116" s="6"/>
     </row>
-    <row r="117" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>3</v>
       </c>
@@ -10116,7 +10146,7 @@
       <c r="Q117" s="3"/>
       <c r="R117" s="3"/>
     </row>
-    <row r="118" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>4</v>
       </c>
@@ -10173,7 +10203,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>4</v>
       </c>
@@ -10224,7 +10254,7 @@
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
     </row>
-    <row r="120" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>4</v>
       </c>
@@ -10275,7 +10305,7 @@
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
     </row>
-    <row r="121" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>4</v>
       </c>
@@ -10326,7 +10356,7 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
     </row>
-    <row r="122" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>1</v>
       </c>
@@ -10377,7 +10407,7 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="1:18" ht="66" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>1</v>
       </c>
@@ -10428,7 +10458,7 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>1</v>
       </c>
@@ -10479,7 +10509,7 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>2</v>
       </c>
@@ -10530,7 +10560,7 @@
       <c r="Q125" s="3"/>
       <c r="R125" s="3"/>
     </row>
-    <row r="126" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>2</v>
       </c>
@@ -10581,7 +10611,7 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
     </row>
-    <row r="127" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>2</v>
       </c>
@@ -10632,7 +10662,7 @@
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>2</v>
       </c>
@@ -10683,7 +10713,7 @@
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
     </row>
-    <row r="129" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>2</v>
       </c>
@@ -10734,7 +10764,7 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>2</v>
       </c>
@@ -10785,7 +10815,7 @@
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
     </row>
-    <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
         <v>3</v>
       </c>
@@ -10836,7 +10866,7 @@
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
     </row>
-    <row r="132" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A132" s="10">
         <v>3</v>
       </c>
@@ -10887,7 +10917,7 @@
       <c r="Q132" s="10"/>
       <c r="R132" s="10"/>
     </row>
-    <row r="133" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A133" s="4">
         <v>3</v>
       </c>
@@ -10938,7 +10968,7 @@
       <c r="Q133" s="4"/>
       <c r="R133" s="4"/>
     </row>
-    <row r="134" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>3</v>
       </c>
@@ -10989,7 +11019,7 @@
       <c r="Q134" s="3"/>
       <c r="R134" s="3"/>
     </row>
-    <row r="135" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>3</v>
       </c>
@@ -11040,7 +11070,7 @@
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
     </row>
-    <row r="136" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>4</v>
       </c>
@@ -11091,7 +11121,7 @@
       <c r="Q136" s="2"/>
       <c r="R136" s="2"/>
     </row>
-    <row r="137" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>4</v>
       </c>
@@ -11142,7 +11172,7 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>4</v>
       </c>
@@ -11193,7 +11223,7 @@
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>4</v>
       </c>
@@ -11244,7 +11274,7 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>1</v>
       </c>
@@ -11295,7 +11325,7 @@
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
     </row>
-    <row r="141" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>2</v>
       </c>
@@ -11346,7 +11376,7 @@
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
     </row>
-    <row r="142" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>3</v>
       </c>
@@ -11397,7 +11427,7 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
     </row>
-    <row r="143" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>1</v>
       </c>
@@ -11448,7 +11478,7 @@
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144" s="5">
         <v>1</v>
       </c>
@@ -11499,7 +11529,7 @@
       <c r="Q144" s="5"/>
       <c r="R144" s="5"/>
     </row>
-    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
         <v>4</v>
       </c>
@@ -11550,7 +11580,7 @@
       <c r="Q145" s="4"/>
       <c r="R145" s="4"/>
     </row>
-    <row r="146" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>2</v>
       </c>
@@ -11601,7 +11631,7 @@
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>1</v>
       </c>
@@ -11652,7 +11682,7 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>6</v>
       </c>
@@ -11703,7 +11733,7 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>5</v>
       </c>
@@ -11754,7 +11784,7 @@
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>4</v>
       </c>
@@ -11805,7 +11835,7 @@
       <c r="Q150" s="1"/>
       <c r="R150" s="1"/>
     </row>
-    <row r="151" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>1</v>
       </c>
@@ -11856,7 +11886,7 @@
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152" s="4">
         <v>4</v>
       </c>
@@ -11913,7 +11943,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>3</v>
       </c>
@@ -11964,7 +11994,7 @@
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
     </row>
-    <row r="154" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>4</v>
       </c>
@@ -12015,7 +12045,7 @@
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
     </row>
-    <row r="155" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>3</v>
       </c>
@@ -12066,7 +12096,7 @@
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
     </row>
-    <row r="156" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>1</v>
       </c>
@@ -12117,7 +12147,7 @@
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
     </row>
-    <row r="157" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>1</v>
       </c>
@@ -12168,7 +12198,7 @@
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A158" s="5">
         <v>2</v>
       </c>
@@ -12219,7 +12249,7 @@
       <c r="Q158" s="5"/>
       <c r="R158" s="5"/>
     </row>
-    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A159" s="5">
         <v>2</v>
       </c>
@@ -12276,7 +12306,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="1:18" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:18" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>3</v>
       </c>
@@ -12327,7 +12357,7 @@
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
     </row>
-    <row r="161" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>2</v>
       </c>
@@ -12378,7 +12408,7 @@
       <c r="Q161" s="1"/>
       <c r="R161" s="1"/>
     </row>
-    <row r="162" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>2</v>
       </c>
@@ -12429,7 +12459,7 @@
       <c r="Q162" s="1"/>
       <c r="R162" s="1"/>
     </row>
-    <row r="163" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>1</v>
       </c>
@@ -12480,7 +12510,7 @@
       <c r="Q163" s="1"/>
       <c r="R163" s="1"/>
     </row>
-    <row r="164" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>1</v>
       </c>
@@ -12531,7 +12561,7 @@
       <c r="Q164" s="1"/>
       <c r="R164" s="1"/>
     </row>
-    <row r="165" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>4</v>
       </c>
@@ -12582,7 +12612,7 @@
       <c r="Q165" s="1"/>
       <c r="R165" s="1"/>
     </row>
-    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>1</v>
       </c>
@@ -12633,7 +12663,7 @@
       <c r="Q166" s="1"/>
       <c r="R166" s="1"/>
     </row>
-    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A167" s="6">
         <v>6</v>
       </c>
@@ -12684,7 +12714,7 @@
       <c r="Q167" s="6"/>
       <c r="R167" s="6"/>
     </row>
-    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>3</v>
       </c>
@@ -12735,7 +12765,7 @@
       <c r="Q168" s="1"/>
       <c r="R168" s="1"/>
     </row>
-    <row r="169" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>4</v>
       </c>
@@ -12786,7 +12816,7 @@
       <c r="Q169" s="1"/>
       <c r="R169" s="1"/>
     </row>
-    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A170" s="6">
         <v>6</v>
       </c>
@@ -12843,7 +12873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>3</v>
       </c>
@@ -12894,7 +12924,7 @@
       <c r="Q171" s="1"/>
       <c r="R171" s="1"/>
     </row>
-    <row r="172" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>3</v>
       </c>
@@ -12945,7 +12975,7 @@
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
     </row>
-    <row r="173" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>3</v>
       </c>
@@ -12996,7 +13026,7 @@
       <c r="Q173" s="1"/>
       <c r="R173" s="1"/>
     </row>
-    <row r="174" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>3</v>
       </c>
@@ -13047,7 +13077,7 @@
       <c r="Q174" s="1"/>
       <c r="R174" s="1"/>
     </row>
-    <row r="175" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>3</v>
       </c>
@@ -13098,7 +13128,7 @@
       <c r="Q175" s="1"/>
       <c r="R175" s="1"/>
     </row>
-    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>4</v>
       </c>
@@ -13149,7 +13179,7 @@
       <c r="Q176" s="1"/>
       <c r="R176" s="1"/>
     </row>
-    <row r="177" spans="1:18" ht="99" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:18" ht="99" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>4</v>
       </c>
@@ -13200,7 +13230,7 @@
       <c r="Q177" s="1"/>
       <c r="R177" s="1"/>
     </row>
-    <row r="178" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>4</v>
       </c>
@@ -13251,7 +13281,7 @@
       <c r="Q178" s="1"/>
       <c r="R178" s="1"/>
     </row>
-    <row r="179" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>4</v>
       </c>
@@ -13302,7 +13332,7 @@
       <c r="Q179" s="1"/>
       <c r="R179" s="1"/>
     </row>
-    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A180" s="5">
         <v>5</v>
       </c>
@@ -13353,7 +13383,7 @@
       <c r="Q180" s="5"/>
       <c r="R180" s="5"/>
     </row>
-    <row r="181" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>1</v>
       </c>
@@ -13404,7 +13434,7 @@
       <c r="Q181" s="1"/>
       <c r="R181" s="1"/>
     </row>
-    <row r="182" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>1</v>
       </c>
@@ -13455,7 +13485,7 @@
       <c r="Q182" s="1"/>
       <c r="R182" s="1"/>
     </row>
-    <row r="183" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>1</v>
       </c>
@@ -13506,7 +13536,7 @@
       <c r="Q183" s="1"/>
       <c r="R183" s="1"/>
     </row>
-    <row r="184" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>1</v>
       </c>
@@ -13557,7 +13587,7 @@
       <c r="Q184" s="1"/>
       <c r="R184" s="1"/>
     </row>
-    <row r="185" spans="1:18" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:18" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>1</v>
       </c>
@@ -13608,7 +13638,7 @@
       <c r="Q185" s="1"/>
       <c r="R185" s="1"/>
     </row>
-    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>2</v>
       </c>
@@ -13659,7 +13689,7 @@
       <c r="Q186" s="1"/>
       <c r="R186" s="1"/>
     </row>
-    <row r="187" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>2</v>
       </c>
@@ -13710,7 +13740,7 @@
       <c r="Q187" s="1"/>
       <c r="R187" s="1"/>
     </row>
-    <row r="188" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>2</v>
       </c>
@@ -13761,7 +13791,7 @@
       <c r="Q188" s="1"/>
       <c r="R188" s="1"/>
     </row>
-    <row r="189" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>2</v>
       </c>
@@ -13812,7 +13842,7 @@
       <c r="Q189" s="1"/>
       <c r="R189" s="1"/>
     </row>
-    <row r="190" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>2</v>
       </c>
@@ -13863,7 +13893,7 @@
       <c r="Q190" s="1"/>
       <c r="R190" s="1"/>
     </row>
-    <row r="191" spans="1:18" ht="66" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>2</v>
       </c>
@@ -13914,7 +13944,7 @@
       <c r="Q191" s="1"/>
       <c r="R191" s="1"/>
     </row>
-    <row r="192" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>1</v>
       </c>
@@ -13965,7 +13995,7 @@
       <c r="Q192" s="1"/>
       <c r="R192" s="1"/>
     </row>
-    <row r="193" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>1</v>
       </c>
@@ -14016,7 +14046,7 @@
       <c r="Q193" s="1"/>
       <c r="R193" s="1"/>
     </row>
-    <row r="194" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>1</v>
       </c>
@@ -14067,7 +14097,7 @@
       <c r="Q194" s="1"/>
       <c r="R194" s="1"/>
     </row>
-    <row r="195" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>1</v>
       </c>
@@ -14118,7 +14148,7 @@
       <c r="Q195" s="1"/>
       <c r="R195" s="1"/>
     </row>
-    <row r="196" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>1</v>
       </c>
@@ -14169,7 +14199,7 @@
       <c r="Q196" s="1"/>
       <c r="R196" s="1"/>
     </row>
-    <row r="197" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>2</v>
       </c>
@@ -14220,7 +14250,7 @@
       <c r="Q197" s="1"/>
       <c r="R197" s="1"/>
     </row>
-    <row r="198" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>2</v>
       </c>
@@ -14271,7 +14301,7 @@
       <c r="Q198" s="1"/>
       <c r="R198" s="1"/>
     </row>
-    <row r="199" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>2</v>
       </c>
@@ -14322,7 +14352,7 @@
       <c r="Q199" s="1"/>
       <c r="R199" s="1"/>
     </row>
-    <row r="200" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>2</v>
       </c>
@@ -14373,7 +14403,7 @@
       <c r="Q200" s="1"/>
       <c r="R200" s="1"/>
     </row>
-    <row r="201" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>2</v>
       </c>
@@ -14424,7 +14454,7 @@
       <c r="Q201" s="1"/>
       <c r="R201" s="1"/>
     </row>
-    <row r="202" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>2</v>
       </c>
@@ -15036,7 +15066,7 @@
       <c r="Q213" s="1"/>
       <c r="R213" s="1"/>
     </row>
-    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A214" s="5">
         <v>1</v>
       </c>
@@ -15093,7 +15123,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>1</v>
       </c>
@@ -15144,7 +15174,7 @@
       <c r="Q215" s="1"/>
       <c r="R215" s="1"/>
     </row>
-    <row r="216" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>1</v>
       </c>
@@ -15195,7 +15225,7 @@
       <c r="Q216" s="1"/>
       <c r="R216" s="1"/>
     </row>
-    <row r="217" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>1</v>
       </c>
@@ -15246,7 +15276,7 @@
       <c r="Q217" s="1"/>
       <c r="R217" s="1"/>
     </row>
-    <row r="218" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>1</v>
       </c>
@@ -15297,7 +15327,7 @@
       <c r="Q218" s="1"/>
       <c r="R218" s="1"/>
     </row>
-    <row r="219" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>1</v>
       </c>
@@ -15348,7 +15378,7 @@
       <c r="Q219" s="1"/>
       <c r="R219" s="1"/>
     </row>
-    <row r="220" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>1</v>
       </c>
@@ -15399,7 +15429,7 @@
       <c r="Q220" s="1"/>
       <c r="R220" s="1"/>
     </row>
-    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>2</v>
       </c>
@@ -15450,7 +15480,7 @@
       <c r="Q221" s="1"/>
       <c r="R221" s="1"/>
     </row>
-    <row r="222" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>2</v>
       </c>
@@ -15501,7 +15531,7 @@
       <c r="Q222" s="1"/>
       <c r="R222" s="1"/>
     </row>
-    <row r="223" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>2</v>
       </c>
@@ -15552,7 +15582,7 @@
       <c r="Q223" s="1"/>
       <c r="R223" s="1"/>
     </row>
-    <row r="224" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>2</v>
       </c>
@@ -15603,7 +15633,7 @@
       <c r="Q224" s="1"/>
       <c r="R224" s="1"/>
     </row>
-    <row r="225" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>2</v>
       </c>
@@ -15654,7 +15684,7 @@
       <c r="Q225" s="1"/>
       <c r="R225" s="1"/>
     </row>
-    <row r="226" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>2</v>
       </c>
@@ -15705,7 +15735,7 @@
       <c r="Q226" s="1"/>
       <c r="R226" s="1"/>
     </row>
-    <row r="227" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>2</v>
       </c>
@@ -15756,7 +15786,7 @@
       <c r="Q227" s="1"/>
       <c r="R227" s="1"/>
     </row>
-    <row r="228" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>4</v>
       </c>
@@ -15807,7 +15837,7 @@
       <c r="Q228" s="1"/>
       <c r="R228" s="1"/>
     </row>
-    <row r="229" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A229" s="4">
         <v>3</v>
       </c>
@@ -15858,7 +15888,7 @@
       <c r="Q229" s="4"/>
       <c r="R229" s="4"/>
     </row>
-    <row r="230" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A230" s="3">
         <v>1</v>
       </c>
@@ -15909,7 +15939,7 @@
       <c r="Q230" s="3"/>
       <c r="R230" s="3"/>
     </row>
-    <row r="231" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>2</v>
       </c>
@@ -15960,7 +15990,7 @@
       <c r="Q231" s="1"/>
       <c r="R231" s="1"/>
     </row>
-    <row r="232" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>1</v>
       </c>
@@ -16011,7 +16041,7 @@
       <c r="Q232" s="1"/>
       <c r="R232" s="1"/>
     </row>
-    <row r="233" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>1</v>
       </c>
@@ -16062,7 +16092,7 @@
       <c r="Q233" s="1"/>
       <c r="R233" s="1"/>
     </row>
-    <row r="234" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A234" s="4">
         <v>1</v>
       </c>
@@ -16113,7 +16143,7 @@
       <c r="Q234" s="4"/>
       <c r="R234" s="4"/>
     </row>
-    <row r="235" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>2</v>
       </c>
@@ -16164,7 +16194,7 @@
       <c r="Q235" s="1"/>
       <c r="R235" s="1"/>
     </row>
-    <row r="236" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>2</v>
       </c>
@@ -16215,7 +16245,7 @@
       <c r="Q236" s="1"/>
       <c r="R236" s="1"/>
     </row>
-    <row r="237" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>4</v>
       </c>
@@ -16266,7 +16296,7 @@
       <c r="Q237" s="1"/>
       <c r="R237" s="1"/>
     </row>
-    <row r="238" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>4</v>
       </c>
@@ -16317,7 +16347,7 @@
       <c r="Q238" s="1"/>
       <c r="R238" s="1"/>
     </row>
-    <row r="239" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A239" s="6">
         <v>3</v>
       </c>
@@ -16368,7 +16398,7 @@
       <c r="Q239" s="6"/>
       <c r="R239" s="6"/>
     </row>
-    <row r="240" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A240" s="5">
         <v>1</v>
       </c>
@@ -16419,7 +16449,7 @@
       <c r="Q240" s="5"/>
       <c r="R240" s="5"/>
     </row>
-    <row r="241" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A241" s="10">
         <v>2</v>
       </c>
@@ -16470,7 +16500,7 @@
       <c r="Q241" s="10"/>
       <c r="R241" s="10"/>
     </row>
-    <row r="242" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>2</v>
       </c>
@@ -16521,7 +16551,7 @@
       <c r="Q242" s="1"/>
       <c r="R242" s="1"/>
     </row>
-    <row r="243" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A243" s="10">
         <v>3</v>
       </c>
@@ -16572,7 +16602,7 @@
       <c r="Q243" s="10"/>
       <c r="R243" s="10"/>
     </row>
-    <row r="244" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>3</v>
       </c>
@@ -16623,7 +16653,7 @@
       <c r="Q244" s="1"/>
       <c r="R244" s="1"/>
     </row>
-    <row r="245" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A245" s="10">
         <v>4</v>
       </c>
@@ -16674,7 +16704,7 @@
       <c r="Q245" s="10"/>
       <c r="R245" s="10"/>
     </row>
-    <row r="246" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>4</v>
       </c>
@@ -16725,7 +16755,7 @@
       <c r="Q246" s="1"/>
       <c r="R246" s="1"/>
     </row>
-    <row r="247" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A247" s="6">
         <v>3</v>
       </c>
@@ -16776,7 +16806,7 @@
       <c r="Q247" s="6"/>
       <c r="R247" s="6"/>
     </row>
-    <row r="248" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A248" s="5">
         <v>5</v>
       </c>
@@ -16833,7 +16863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A249" s="6">
         <v>3</v>
       </c>
@@ -16890,7 +16920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="250" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A250" s="3">
         <v>3</v>
       </c>
@@ -16947,7 +16977,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="251" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A251" s="6">
         <v>3</v>
       </c>
@@ -17004,7 +17034,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="252" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A252" s="3">
         <v>3</v>
       </c>
@@ -17061,7 +17091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="253" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A253" s="6">
         <v>3</v>
       </c>
@@ -17118,7 +17148,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="254" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A254" s="6">
         <v>3</v>
       </c>
@@ -17175,7 +17205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="255" spans="1:18" ht="66" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A255" s="4">
         <v>3</v>
       </c>
@@ -17232,7 +17262,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="256" spans="1:18" ht="66" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A256" s="4">
         <v>3</v>
       </c>
@@ -17289,7 +17319,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="257" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A257" s="10">
         <v>1</v>
       </c>
@@ -17346,7 +17376,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="258" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A258" s="4">
         <v>3</v>
       </c>
@@ -17403,7 +17433,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="259" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A259" s="4">
         <v>3</v>
       </c>
@@ -17460,7 +17490,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="260" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A260" s="3">
         <v>3</v>
       </c>
@@ -17517,7 +17547,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="261" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A261" s="3">
         <v>3</v>
       </c>
@@ -17574,7 +17604,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="262" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A262" s="12">
         <v>3</v>
       </c>
@@ -17631,7 +17661,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="263" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263" s="12">
         <v>3</v>
       </c>
@@ -17688,7 +17718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="264" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A264" s="32">
         <v>3</v>
       </c>
@@ -17745,7 +17775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="265" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265" s="12">
         <v>1</v>
       </c>
@@ -17802,7 +17832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="266" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A266" s="6">
         <v>5</v>
       </c>
@@ -17859,7 +17889,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="267" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A267" s="6">
         <v>6</v>
       </c>
@@ -17916,7 +17946,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="268" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A268" s="5">
         <v>1</v>
       </c>
@@ -17973,7 +18003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="269" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A269" s="5">
         <v>1</v>
       </c>
@@ -18030,7 +18060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="270" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A270" s="5">
         <v>1</v>
       </c>
@@ -18258,7 +18288,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="274" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A274" s="3">
         <v>3</v>
       </c>
@@ -18315,7 +18345,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="275" spans="1:18" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:18" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A275" s="3">
         <v>3</v>
       </c>
@@ -18372,7 +18402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="276" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A276" s="6">
         <v>6</v>
       </c>
@@ -18429,7 +18459,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="277" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A277" s="6">
         <v>4</v>
       </c>
@@ -18486,7 +18516,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="278" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A278" s="22">
         <v>3</v>
       </c>
@@ -18543,7 +18573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="279" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A279" s="24">
         <v>3</v>
       </c>
@@ -18600,7 +18630,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="280" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A280" s="26">
         <v>4</v>
       </c>
@@ -18657,7 +18687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="281" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A281" s="24">
         <v>3</v>
       </c>
@@ -18714,7 +18744,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="282" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A282" s="22">
         <v>3</v>
       </c>
@@ -18771,7 +18801,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="283" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A283" s="28">
         <v>3</v>
       </c>
@@ -18828,7 +18858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="284" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A284" s="30">
         <v>1</v>
       </c>
@@ -18885,7 +18915,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="285" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A285" s="26">
         <v>3</v>
       </c>
@@ -18942,7 +18972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="286" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A286" s="32">
         <v>3</v>
       </c>
@@ -18999,7 +19029,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="287" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A287" s="26">
         <v>3</v>
       </c>
@@ -19056,7 +19086,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="288" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A288" s="30">
         <v>3</v>
       </c>
@@ -19113,7 +19143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="289" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A289" s="30">
         <v>3</v>
       </c>
@@ -19170,7 +19200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="290" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A290" s="24">
         <v>3</v>
       </c>
@@ -19227,7 +19257,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="291" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A291" s="24">
         <v>3</v>
       </c>
@@ -19284,7 +19314,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="292" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A292" s="22">
         <v>1</v>
       </c>
@@ -19341,7 +19371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="293" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A293" s="24">
         <v>4</v>
       </c>
@@ -19398,7 +19428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="294" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A294" s="22">
         <v>4</v>
       </c>
@@ -19455,7 +19485,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="295" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A295" s="22">
         <v>1</v>
       </c>
@@ -19512,7 +19542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="296" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A296" s="26">
         <v>2</v>
       </c>
@@ -19569,7 +19599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="297" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A297" s="32">
         <v>2</v>
       </c>
@@ -19626,7 +19656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="298" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A298" s="32">
         <v>2</v>
       </c>
@@ -19683,7 +19713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="299" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A299" s="26">
         <v>1</v>
       </c>
@@ -19740,7 +19770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="300" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A300" s="28">
         <v>3</v>
       </c>
@@ -19797,7 +19827,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="301" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A301" s="22">
         <v>3</v>
       </c>
@@ -19854,7 +19884,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="302" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A302" s="22">
         <v>1</v>
       </c>
@@ -19911,7 +19941,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="303" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A303" s="28">
         <v>1</v>
       </c>
@@ -19968,7 +19998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="304" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A304" s="30">
         <v>1</v>
       </c>
@@ -20025,7 +20055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="305" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A305" s="24">
         <v>2</v>
       </c>
@@ -20082,7 +20112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="306" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A306" s="26">
         <v>2</v>
       </c>
@@ -20139,7 +20169,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="307" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A307" s="30">
         <v>2</v>
       </c>
@@ -20196,7 +20226,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="308" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A308" s="22">
         <v>2</v>
       </c>
@@ -20253,7 +20283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="309" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A309" s="32">
         <v>4</v>
       </c>
@@ -20310,7 +20340,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="310" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A310" s="22">
         <v>4</v>
       </c>
@@ -20367,7 +20397,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="311" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A311" s="32">
         <v>4</v>
       </c>
@@ -20424,7 +20454,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="312" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A312" s="26">
         <v>4</v>
       </c>
@@ -20481,7 +20511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="313" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A313" s="28">
         <v>3</v>
       </c>
@@ -20538,7 +20568,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="314" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A314" s="32">
         <v>1</v>
       </c>
@@ -20595,7 +20625,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="315" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A315" s="22">
         <v>1</v>
       </c>
@@ -20652,7 +20682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="316" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A316" s="24">
         <v>1</v>
       </c>
@@ -20709,7 +20739,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="317" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A317" s="26">
         <v>3</v>
       </c>
@@ -20766,7 +20796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="318" spans="1:18" ht="33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A318" s="22">
         <v>3</v>
       </c>
@@ -20823,7 +20853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="319" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A319" s="26">
         <v>3</v>
       </c>
@@ -20880,7 +20910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="320" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A320" s="28">
         <v>2</v>
       </c>
@@ -20937,7 +20967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="321" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A321" s="28">
         <v>4</v>
       </c>
@@ -20994,7 +21024,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="322" spans="1:18" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:18" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A322" s="24">
         <v>3</v>
       </c>
@@ -21051,7 +21081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="323" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A323" s="24">
         <v>2</v>
       </c>
@@ -21108,7 +21138,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="324" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A324" s="22">
         <v>3</v>
       </c>
@@ -21164,6 +21194,159 @@
       <c r="R324" s="22" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="325" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+      <c r="A325" s="1">
+        <v>2</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D325" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E325" s="1">
+        <v>1</v>
+      </c>
+      <c r="F325" s="15" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G325" s="1" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H325" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="I325" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="J325" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K325" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="L325" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="M325" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N325" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="O325" t="s">
+        <v>23</v>
+      </c>
+      <c r="P325" s="1"/>
+      <c r="Q325" s="1"/>
+      <c r="R325" s="1"/>
+    </row>
+    <row r="326" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+      <c r="A326" s="1">
+        <v>1</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E326" s="1">
+        <v>1</v>
+      </c>
+      <c r="F326" s="15" t="s">
+        <v>1164</v>
+      </c>
+      <c r="G326" s="1" t="s">
+        <v>1165</v>
+      </c>
+      <c r="H326" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="I326" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="J326" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="K326" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="L326" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="M326" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N326" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="O326" t="s">
+        <v>23</v>
+      </c>
+      <c r="P326" s="1"/>
+      <c r="Q326" s="1"/>
+      <c r="R326" s="1"/>
+    </row>
+    <row r="327" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+      <c r="A327" s="1">
+        <v>1</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="E327" s="1">
+        <v>1</v>
+      </c>
+      <c r="F327" s="15" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G327" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="H327" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="I327" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="J327" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="K327" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="L327" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="M327" s="22" t="b">
+        <f>NOT(ISBLANK(Table1[[#This Row],[codigo_de_asignatura_de_referencia]]))</f>
+        <v>0</v>
+      </c>
+      <c r="N327" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="O327" t="s">
+        <v>23</v>
+      </c>
+      <c r="P327" s="1"/>
+      <c r="Q327" s="1"/>
+      <c r="R327" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>